<commit_message>
system 5 and 3 spreadsheet
</commit_message>
<xml_diff>
--- a/projects/office_calibration_rgenoud_14_Sys5.xlsx
+++ b/projects/office_calibration_rgenoud_14_Sys5.xlsx
@@ -7318,9 +7318,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y231"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q87" sqref="Q87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -9365,7 +9365,7 @@
       </c>
       <c r="P87" s="47"/>
       <c r="Q87" s="43" t="s">
-        <v>24</v>
+        <v>754</v>
       </c>
     </row>
     <row r="88" spans="1:17">

</xml_diff>

<commit_message>
update outputs on all spreadsheets and remove unneeded ones
</commit_message>
<xml_diff>
--- a/projects/office_calibration_rgenoud_14_Sys5.xlsx
+++ b/projects/office_calibration_rgenoud_14_Sys5.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="13170" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="27640" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="TrueFalse">Lookups!$C$12:$C$13</definedName>
     <definedName name="Workflow">Lookups!$E$12:$E$13</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2614" uniqueCount="828">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2686" uniqueCount="866">
   <si>
     <t>type</t>
   </si>
@@ -2525,6 +2525,120 @@
   </si>
   <si>
     <t>Add Sys 5 PVAV Ngrid</t>
+  </si>
+  <si>
+    <t>Natural Gas Heating Intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.heating_natural_gas</t>
+  </si>
+  <si>
+    <t>Cooling Electricity Intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.cooling_electricity</t>
+  </si>
+  <si>
+    <t>Interior Lighting Electricity Intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.interior_lighting_electricity</t>
+  </si>
+  <si>
+    <t>Exterior Lighting Electricity Intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.exterior_lighting_electricity</t>
+  </si>
+  <si>
+    <t>Equipment Electricity Intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.interior_equipment_electricity</t>
+  </si>
+  <si>
+    <t>Equipment Natural Gas Intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.interior_equipment_natural_gas</t>
+  </si>
+  <si>
+    <t>Experior Equipment Electricity Intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.exterior_equipment_electricity</t>
+  </si>
+  <si>
+    <t>Fans Electricity Intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.fans_electricity</t>
+  </si>
+  <si>
+    <t>Pumps Electricity Intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.pumps_electricity</t>
+  </si>
+  <si>
+    <t>Heat Rejection Electricity Intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.heat_rejection_electricity</t>
+  </si>
+  <si>
+    <t>Humidification Electricity Intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.humidification_electricity</t>
+  </si>
+  <si>
+    <t>Water Systems Electricity Intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.water_systems_electricity</t>
+  </si>
+  <si>
+    <t>Water Systems Natural Gas Intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.water_systems_natural_gas</t>
+  </si>
+  <si>
+    <t>Refrigeration Electricity Intensity</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.refrigeration_electricity</t>
+  </si>
+  <si>
+    <t>Unmet Cooling Hours</t>
+  </si>
+  <si>
+    <t>standard_report.time_setpoint_not_met_during_occupied_cooling</t>
+  </si>
+  <si>
+    <t>hrs</t>
+  </si>
+  <si>
+    <t>Unmet Heating Hours</t>
+  </si>
+  <si>
+    <t>standard_report.time_setpoint_not_met_during_occupied_heating</t>
+  </si>
+  <si>
+    <t>Total Unmet Hours</t>
+  </si>
+  <si>
+    <t>standard_report.time_setpoint_not_met_during_occupied_hours</t>
+  </si>
+  <si>
+    <t>Building Area</t>
+  </si>
+  <si>
+    <t>standard_report.total_building_area</t>
+  </si>
+  <si>
+    <t>m2</t>
   </si>
 </sst>
 </file>
@@ -2534,7 +2648,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4536,7 +4650,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -4640,6 +4754,7 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6785,17 +6900,17 @@
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="81.7109375" customWidth="1"/>
+    <col min="1" max="1" width="81.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="45">
+    <row r="1" spans="1:1" ht="28">
       <c r="A1" s="36" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="30">
+    <row r="2" spans="1:1" ht="28">
       <c r="A2" s="36" t="s">
         <v>41</v>
       </c>
@@ -6819,14 +6934,14 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" style="26" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" style="1" customWidth="1"/>
-    <col min="4" max="4" width="33.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="61.7109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.7109375" style="1"/>
+    <col min="4" max="4" width="33.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="61.6640625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -6858,7 +6973,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30">
+    <row r="4" spans="1:5" ht="28">
       <c r="A4" s="1" t="s">
         <v>456</v>
       </c>
@@ -6869,7 +6984,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="75">
+    <row r="5" spans="1:5" ht="42">
       <c r="A5" s="1" t="s">
         <v>469</v>
       </c>
@@ -6880,7 +6995,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="46.15" customHeight="1">
+    <row r="6" spans="1:5" ht="46.25" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>470</v>
       </c>
@@ -6891,7 +7006,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30">
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>442</v>
       </c>
@@ -6910,7 +7025,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30">
+    <row r="8" spans="1:5" ht="28">
       <c r="A8" s="1" t="s">
         <v>443</v>
       </c>
@@ -6995,7 +7110,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30">
+    <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
         <v>463</v>
       </c>
@@ -7028,7 +7143,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="2" customFormat="1" ht="60">
+    <row r="20" spans="1:5" s="2" customFormat="1" ht="42">
       <c r="A20" s="11" t="s">
         <v>27</v>
       </c>
@@ -7053,7 +7168,7 @@
       <c r="B22" s="26"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:5" s="2" customFormat="1" ht="60">
+    <row r="23" spans="1:5" s="2" customFormat="1" ht="42">
       <c r="A23" s="11" t="s">
         <v>450</v>
       </c>
@@ -7212,7 +7327,7 @@
       </c>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:5" s="2" customFormat="1" ht="45">
+    <row r="36" spans="1:5" s="2" customFormat="1" ht="28">
       <c r="A36" s="11" t="s">
         <v>33</v>
       </c>
@@ -7233,7 +7348,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="2" customFormat="1" ht="30">
+    <row r="39" spans="1:5" s="2" customFormat="1" ht="28">
       <c r="A39" s="11" t="s">
         <v>30</v>
       </c>
@@ -7262,7 +7377,7 @@
       </c>
       <c r="E40" s="2"/>
     </row>
-    <row r="42" spans="1:5" s="2" customFormat="1" ht="60">
+    <row r="42" spans="1:5" s="2" customFormat="1" ht="56">
       <c r="A42" s="11" t="s">
         <v>35</v>
       </c>
@@ -7318,37 +7433,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H114" sqref="H114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="31" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" style="31" customWidth="1"/>
     <col min="2" max="2" width="47" style="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47" style="31" customWidth="1"/>
-    <col min="4" max="4" width="39.140625" style="31" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" style="31" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="31" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="31" customWidth="1"/>
-    <col min="11" max="11" width="8.140625" style="31" customWidth="1"/>
-    <col min="12" max="12" width="6.7109375" style="31" customWidth="1"/>
-    <col min="13" max="14" width="7.7109375" style="31" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" style="31"/>
-    <col min="16" max="16" width="11.42578125" style="31" customWidth="1"/>
+    <col min="4" max="4" width="39.1640625" style="31" customWidth="1"/>
+    <col min="5" max="5" width="24.1640625" style="31" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" style="31" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5" style="4" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="7.1640625" style="31" customWidth="1"/>
+    <col min="11" max="11" width="8.1640625" style="31" customWidth="1"/>
+    <col min="12" max="12" width="6.6640625" style="31" customWidth="1"/>
+    <col min="13" max="14" width="7.6640625" style="31" customWidth="1"/>
+    <col min="15" max="15" width="11.5" style="31"/>
+    <col min="16" max="16" width="11.5" style="31" customWidth="1"/>
     <col min="17" max="17" width="23" style="31" customWidth="1"/>
-    <col min="18" max="18" width="27.7109375" style="31" customWidth="1"/>
-    <col min="19" max="19" width="46.140625" style="31" customWidth="1"/>
-    <col min="20" max="22" width="11.42578125" style="31"/>
-    <col min="23" max="23" width="13.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="11.42578125" style="31"/>
+    <col min="18" max="18" width="27.6640625" style="31" customWidth="1"/>
+    <col min="19" max="19" width="46.1640625" style="31" customWidth="1"/>
+    <col min="20" max="22" width="11.5" style="31"/>
+    <col min="23" max="23" width="13.33203125" style="31" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="11.5" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="18.75">
+    <row r="1" spans="1:25" ht="18">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -7374,16 +7489,16 @@
       <c r="Q1" s="5"/>
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
-      <c r="T1" s="53" t="s">
+      <c r="T1" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
-    </row>
-    <row r="2" spans="1:25" s="8" customFormat="1" ht="15.75">
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+    </row>
+    <row r="2" spans="1:25" s="8" customFormat="1" ht="15">
       <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
@@ -7399,7 +7514,7 @@
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
     </row>
-    <row r="3" spans="1:25" s="14" customFormat="1" ht="63">
+    <row r="3" spans="1:25" s="14" customFormat="1" ht="45">
       <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
@@ -7666,7 +7781,7 @@
       <c r="G13" s="39"/>
       <c r="H13" s="39"/>
     </row>
-    <row r="14" spans="1:25" ht="18">
+    <row r="14" spans="1:25" ht="17">
       <c r="A14" s="30"/>
       <c r="B14" s="30" t="s">
         <v>21</v>
@@ -10557,27 +10672,27 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="29.42578125" style="31" customWidth="1"/>
+    <col min="1" max="2" width="29.5" style="31" customWidth="1"/>
     <col min="3" max="3" width="71" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="31" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.42578125" style="31" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="31" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" style="31" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" style="31" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="31"/>
+    <col min="4" max="4" width="10.5" style="31" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.5" style="31" customWidth="1"/>
+    <col min="8" max="8" width="14.5" style="31" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" style="31" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" style="31" customWidth="1"/>
+    <col min="11" max="16384" width="11.5" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.75">
+    <row r="1" spans="1:12" ht="18">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -10592,7 +10707,7 @@
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
     </row>
-    <row r="2" spans="1:12" s="8" customFormat="1" ht="15.75">
+    <row r="2" spans="1:12" s="8" customFormat="1" ht="15">
       <c r="A2" s="8" t="s">
         <v>459</v>
       </c>
@@ -10627,7 +10742,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="14" customFormat="1" ht="47.25">
+    <row r="3" spans="1:12" s="14" customFormat="1" ht="30">
       <c r="A3" s="14" t="s">
         <v>628</v>
       </c>
@@ -10782,20 +10897,20 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="30" t="s">
-        <v>706</v>
+        <v>828</v>
       </c>
       <c r="B8" s="30"/>
       <c r="C8" s="30" t="s">
-        <v>770</v>
+        <v>829</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>707</v>
+        <v>468</v>
       </c>
       <c r="E8" s="30" t="s">
         <v>64</v>
       </c>
       <c r="F8" s="30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" s="30" t="b">
         <v>1</v>
@@ -10810,20 +10925,20 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="30" t="s">
-        <v>708</v>
+        <v>830</v>
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="30" t="s">
-        <v>771</v>
+        <v>831</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>709</v>
+        <v>468</v>
       </c>
       <c r="E9" s="30" t="s">
         <v>64</v>
       </c>
       <c r="F9" s="30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="30" t="b">
         <v>1</v>
@@ -10838,135 +10953,665 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="30" t="s">
-        <v>796</v>
+        <v>832</v>
       </c>
       <c r="B10" s="30"/>
       <c r="C10" s="30" t="s">
-        <v>792</v>
+        <v>833</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>783</v>
-      </c>
-      <c r="E10" s="31" t="s">
+        <v>468</v>
+      </c>
+      <c r="E10" s="30" t="s">
         <v>64</v>
       </c>
       <c r="F10" s="30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="30" t="b">
         <v>1</v>
       </c>
       <c r="H10" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="I10" s="31">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="30" t="s">
-        <v>797</v>
+        <v>834</v>
       </c>
       <c r="B11" s="30"/>
       <c r="C11" s="30" t="s">
-        <v>793</v>
+        <v>835</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>783</v>
-      </c>
-      <c r="E11" s="31" t="s">
+        <v>468</v>
+      </c>
+      <c r="E11" s="30" t="s">
         <v>64</v>
       </c>
       <c r="F11" s="30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" s="30" t="b">
         <v>1</v>
       </c>
       <c r="H11" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="I11" s="31">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="30" t="s">
-        <v>798</v>
+        <v>836</v>
       </c>
       <c r="B12" s="30"/>
       <c r="C12" s="30" t="s">
-        <v>794</v>
+        <v>837</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>783</v>
-      </c>
-      <c r="E12" s="31" t="s">
+        <v>468</v>
+      </c>
+      <c r="E12" s="30" t="s">
         <v>64</v>
       </c>
       <c r="F12" s="30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" s="30" t="b">
         <v>1</v>
       </c>
       <c r="H12" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="I12" s="31">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="30" t="s">
-        <v>799</v>
+        <v>838</v>
       </c>
       <c r="B13" s="30"/>
       <c r="C13" s="30" t="s">
-        <v>795</v>
+        <v>839</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>783</v>
-      </c>
-      <c r="E13" s="31" t="s">
+        <v>468</v>
+      </c>
+      <c r="E13" s="30" t="s">
         <v>64</v>
       </c>
       <c r="F13" s="30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" s="30" t="b">
         <v>1</v>
       </c>
       <c r="H13" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="30" t="s">
+        <v>840</v>
+      </c>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30" t="s">
+        <v>841</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>468</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="I13" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="30"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
+      <c r="H14" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="30"/>
+      <c r="A15" s="30" t="s">
+        <v>842</v>
+      </c>
       <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
+      <c r="C15" s="30" t="s">
+        <v>843</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>468</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="30"/>
+      <c r="A16" s="30" t="s">
+        <v>844</v>
+      </c>
       <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="30"/>
+      <c r="C16" s="30" t="s">
+        <v>845</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>468</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="30" t="s">
+        <v>846</v>
+      </c>
       <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
+      <c r="C17" s="30" t="s">
+        <v>847</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>468</v>
+      </c>
+      <c r="E17" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="30" t="s">
+        <v>848</v>
+      </c>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30" t="s">
+        <v>849</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>468</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="30" t="s">
+        <v>850</v>
+      </c>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30" t="s">
+        <v>851</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>468</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="30" t="s">
+        <v>852</v>
+      </c>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30" t="s">
+        <v>853</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>468</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="30" t="s">
+        <v>854</v>
+      </c>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30" t="s">
+        <v>855</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>468</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="30" t="s">
+        <v>856</v>
+      </c>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30" t="s">
+        <v>857</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>858</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G22" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="30" t="s">
+        <v>859</v>
+      </c>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30" t="s">
+        <v>860</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>858</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G23" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="30"/>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="30" t="s">
+        <v>861</v>
+      </c>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30" t="s">
+        <v>862</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>858</v>
+      </c>
+      <c r="E24" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="30"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="30" t="s">
+        <v>863</v>
+      </c>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30" t="s">
+        <v>864</v>
+      </c>
+      <c r="D25" s="30" t="s">
+        <v>865</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25" s="30"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="30"/>
+      <c r="L25" s="30"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="30" t="s">
+        <v>706</v>
+      </c>
+      <c r="B26" s="30"/>
+      <c r="C26" s="30" t="s">
+        <v>770</v>
+      </c>
+      <c r="D26" s="30" t="s">
+        <v>707</v>
+      </c>
+      <c r="E26" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="30" t="s">
+        <v>708</v>
+      </c>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30" t="s">
+        <v>771</v>
+      </c>
+      <c r="D27" s="30" t="s">
+        <v>709</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F27" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G27" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="30" t="s">
+        <v>796</v>
+      </c>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30" t="s">
+        <v>792</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>783</v>
+      </c>
+      <c r="E28" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="F28" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G28" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I28" s="31">
+        <v>0</v>
+      </c>
+      <c r="J28" s="30"/>
+      <c r="K28" s="30"/>
+      <c r="L28" s="30"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="30" t="s">
+        <v>797</v>
+      </c>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30" t="s">
+        <v>793</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>783</v>
+      </c>
+      <c r="E29" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="F29" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I29" s="31">
+        <v>0</v>
+      </c>
+      <c r="J29" s="30"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="30"/>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="30" t="s">
+        <v>798</v>
+      </c>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30" t="s">
+        <v>794</v>
+      </c>
+      <c r="D30" s="30" t="s">
+        <v>783</v>
+      </c>
+      <c r="E30" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="F30" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G30" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I30" s="31">
+        <v>0</v>
+      </c>
+      <c r="J30" s="30"/>
+      <c r="K30" s="30"/>
+      <c r="L30" s="30"/>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="30" t="s">
+        <v>799</v>
+      </c>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30" t="s">
+        <v>795</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>783</v>
+      </c>
+      <c r="E31" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="F31" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I31" s="31">
+        <v>0</v>
+      </c>
+      <c r="J31" s="30"/>
+      <c r="K31" s="30"/>
+      <c r="L31" s="30"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="30"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="30"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="30"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="30"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="30"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="30"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="30"/>
+      <c r="B38" s="30"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -10987,19 +11632,19 @@
       <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="80.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="255.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75">
+    <row r="1" spans="1:9" ht="15">
       <c r="A1" s="17" t="b">
         <v>0</v>
       </c>
@@ -11018,7 +11663,7 @@
       <c r="H1" s="17"/>
       <c r="I1" s="17"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75">
+    <row r="2" spans="1:9" ht="15">
       <c r="A2" s="17"/>
       <c r="B2" s="17" t="s">
         <v>21</v>
@@ -11039,7 +11684,7 @@
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75">
+    <row r="3" spans="1:9" ht="15">
       <c r="A3" s="17"/>
       <c r="B3" s="17" t="s">
         <v>21</v>
@@ -11062,7 +11707,7 @@
       </c>
       <c r="I3" s="17"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75">
+    <row r="4" spans="1:9" ht="15">
       <c r="A4" s="17"/>
       <c r="B4" s="17" t="s">
         <v>21</v>
@@ -11085,7 +11730,7 @@
       </c>
       <c r="I4" s="17"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75">
+    <row r="5" spans="1:9" ht="15">
       <c r="A5" s="17"/>
       <c r="B5" s="17" t="s">
         <v>21</v>
@@ -11108,7 +11753,7 @@
       </c>
       <c r="I5" s="17"/>
     </row>
-    <row r="6" spans="1:9" ht="15.75">
+    <row r="6" spans="1:9" ht="15">
       <c r="A6" s="17"/>
       <c r="B6" s="17" t="s">
         <v>21</v>
@@ -11131,7 +11776,7 @@
       </c>
       <c r="I6" s="17"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75">
+    <row r="7" spans="1:9" ht="15">
       <c r="A7" s="17"/>
       <c r="B7" s="17" t="s">
         <v>21</v>
@@ -11154,7 +11799,7 @@
       </c>
       <c r="I7" s="17"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75">
+    <row r="8" spans="1:9" ht="15">
       <c r="A8" s="17"/>
       <c r="B8" s="17" t="s">
         <v>21</v>
@@ -11177,7 +11822,7 @@
       </c>
       <c r="I8" s="17"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75">
+    <row r="9" spans="1:9" ht="15">
       <c r="A9" s="17"/>
       <c r="B9" s="17" t="s">
         <v>21</v>
@@ -11200,7 +11845,7 @@
       </c>
       <c r="I9" s="17"/>
     </row>
-    <row r="10" spans="1:9" ht="15.75">
+    <row r="10" spans="1:9" ht="15">
       <c r="A10" s="17"/>
       <c r="B10" s="17" t="s">
         <v>21</v>
@@ -11223,7 +11868,7 @@
       </c>
       <c r="I10" s="17"/>
     </row>
-    <row r="11" spans="1:9" ht="15.75">
+    <row r="11" spans="1:9" ht="15">
       <c r="A11" s="17" t="b">
         <v>0</v>
       </c>
@@ -11242,7 +11887,7 @@
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75">
+    <row r="12" spans="1:9" ht="15">
       <c r="A12" s="17"/>
       <c r="B12" s="17" t="s">
         <v>21</v>
@@ -11263,7 +11908,7 @@
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
     </row>
-    <row r="13" spans="1:9" ht="15.75">
+    <row r="13" spans="1:9" ht="15">
       <c r="A13" s="17"/>
       <c r="B13" s="17" t="s">
         <v>21</v>
@@ -11286,7 +11931,7 @@
       </c>
       <c r="I13" s="17"/>
     </row>
-    <row r="14" spans="1:9" ht="15.75">
+    <row r="14" spans="1:9" ht="15">
       <c r="A14" s="17"/>
       <c r="B14" s="17" t="s">
         <v>21</v>
@@ -11309,7 +11954,7 @@
       </c>
       <c r="I14" s="17"/>
     </row>
-    <row r="15" spans="1:9" ht="15.75">
+    <row r="15" spans="1:9" ht="15">
       <c r="A15" s="17"/>
       <c r="B15" s="17" t="s">
         <v>21</v>
@@ -11332,7 +11977,7 @@
       </c>
       <c r="I15" s="17"/>
     </row>
-    <row r="16" spans="1:9" ht="15.75">
+    <row r="16" spans="1:9" ht="15">
       <c r="A16" s="17"/>
       <c r="B16" s="17" t="s">
         <v>21</v>
@@ -11355,7 +12000,7 @@
       </c>
       <c r="I16" s="17"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75">
+    <row r="17" spans="1:9" ht="15">
       <c r="A17" s="17"/>
       <c r="B17" s="17" t="s">
         <v>21</v>
@@ -11378,7 +12023,7 @@
       </c>
       <c r="I17" s="17"/>
     </row>
-    <row r="18" spans="1:9" ht="15.75">
+    <row r="18" spans="1:9" ht="15">
       <c r="A18" s="17"/>
       <c r="B18" s="17" t="s">
         <v>21</v>
@@ -11401,7 +12046,7 @@
       </c>
       <c r="I18" s="17"/>
     </row>
-    <row r="19" spans="1:9" ht="15.75">
+    <row r="19" spans="1:9" ht="15">
       <c r="A19" s="17"/>
       <c r="B19" s="17" t="s">
         <v>21</v>
@@ -11424,7 +12069,7 @@
       </c>
       <c r="I19" s="17"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75">
+    <row r="20" spans="1:9" ht="15">
       <c r="A20" s="17"/>
       <c r="B20" s="17" t="s">
         <v>21</v>
@@ -11447,7 +12092,7 @@
       </c>
       <c r="I20" s="17"/>
     </row>
-    <row r="21" spans="1:9" ht="15.75">
+    <row r="21" spans="1:9" ht="15">
       <c r="A21" s="17" t="b">
         <v>0</v>
       </c>
@@ -11466,7 +12111,7 @@
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
     </row>
-    <row r="22" spans="1:9" ht="15.75">
+    <row r="22" spans="1:9" ht="15">
       <c r="A22" s="17"/>
       <c r="B22" s="17" t="s">
         <v>21</v>
@@ -11489,7 +12134,7 @@
       </c>
       <c r="I22" s="17"/>
     </row>
-    <row r="23" spans="1:9" ht="15.75">
+    <row r="23" spans="1:9" ht="15">
       <c r="A23" s="17"/>
       <c r="B23" s="17" t="s">
         <v>21</v>
@@ -11512,7 +12157,7 @@
       </c>
       <c r="I23" s="17"/>
     </row>
-    <row r="24" spans="1:9" ht="15.75">
+    <row r="24" spans="1:9" ht="15">
       <c r="A24" s="17"/>
       <c r="B24" s="17" t="s">
         <v>21</v>
@@ -11535,7 +12180,7 @@
       </c>
       <c r="I24" s="17"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75">
+    <row r="25" spans="1:9" ht="15">
       <c r="A25" s="17"/>
       <c r="B25" s="17" t="s">
         <v>21</v>
@@ -11558,7 +12203,7 @@
       </c>
       <c r="I25" s="17"/>
     </row>
-    <row r="26" spans="1:9" ht="15.75">
+    <row r="26" spans="1:9" ht="15">
       <c r="A26" s="17"/>
       <c r="B26" s="17" t="s">
         <v>21</v>
@@ -11581,7 +12226,7 @@
       </c>
       <c r="I26" s="17"/>
     </row>
-    <row r="27" spans="1:9" ht="15.75">
+    <row r="27" spans="1:9" ht="15">
       <c r="A27" s="17"/>
       <c r="B27" s="17" t="s">
         <v>21</v>
@@ -11604,7 +12249,7 @@
       </c>
       <c r="I27" s="17"/>
     </row>
-    <row r="28" spans="1:9" ht="15.75">
+    <row r="28" spans="1:9" ht="15">
       <c r="A28" s="17"/>
       <c r="B28" s="17" t="s">
         <v>21</v>
@@ -11627,7 +12272,7 @@
       </c>
       <c r="I28" s="17"/>
     </row>
-    <row r="29" spans="1:9" ht="15.75">
+    <row r="29" spans="1:9" ht="15">
       <c r="A29" s="17"/>
       <c r="B29" s="17" t="s">
         <v>21</v>
@@ -11650,7 +12295,7 @@
       </c>
       <c r="I29" s="17"/>
     </row>
-    <row r="30" spans="1:9" ht="15.75">
+    <row r="30" spans="1:9" ht="15">
       <c r="A30" s="17"/>
       <c r="B30" s="17" t="s">
         <v>21</v>
@@ -11673,7 +12318,7 @@
       </c>
       <c r="I30" s="17"/>
     </row>
-    <row r="31" spans="1:9" ht="15.75">
+    <row r="31" spans="1:9" ht="15">
       <c r="A31" s="17" t="b">
         <v>0</v>
       </c>
@@ -11692,7 +12337,7 @@
       <c r="H31" s="17"/>
       <c r="I31" s="17"/>
     </row>
-    <row r="32" spans="1:9" ht="15.75">
+    <row r="32" spans="1:9" ht="15">
       <c r="A32" s="17"/>
       <c r="B32" s="17" t="s">
         <v>21</v>
@@ -11713,7 +12358,7 @@
       <c r="H32" s="17"/>
       <c r="I32" s="17"/>
     </row>
-    <row r="33" spans="1:9" ht="15.75">
+    <row r="33" spans="1:9" ht="15">
       <c r="A33" s="17"/>
       <c r="B33" s="17" t="s">
         <v>21</v>
@@ -11736,7 +12381,7 @@
       </c>
       <c r="I33" s="17"/>
     </row>
-    <row r="34" spans="1:9" ht="15.75">
+    <row r="34" spans="1:9" ht="15">
       <c r="A34" s="17"/>
       <c r="B34" s="17" t="s">
         <v>21</v>
@@ -11759,7 +12404,7 @@
       </c>
       <c r="I34" s="17"/>
     </row>
-    <row r="35" spans="1:9" ht="15.75">
+    <row r="35" spans="1:9" ht="15">
       <c r="A35" s="17"/>
       <c r="B35" s="17" t="s">
         <v>21</v>
@@ -11782,7 +12427,7 @@
       </c>
       <c r="I35" s="17"/>
     </row>
-    <row r="36" spans="1:9" ht="15.75">
+    <row r="36" spans="1:9" ht="15">
       <c r="A36" s="17"/>
       <c r="B36" s="17" t="s">
         <v>21</v>
@@ -11805,7 +12450,7 @@
       </c>
       <c r="I36" s="17"/>
     </row>
-    <row r="37" spans="1:9" ht="15.75">
+    <row r="37" spans="1:9" ht="15">
       <c r="A37" s="17"/>
       <c r="B37" s="17" t="s">
         <v>21</v>
@@ -11828,7 +12473,7 @@
       </c>
       <c r="I37" s="17"/>
     </row>
-    <row r="38" spans="1:9" ht="15.75">
+    <row r="38" spans="1:9" ht="15">
       <c r="A38" s="17"/>
       <c r="B38" s="17" t="s">
         <v>21</v>
@@ -11851,7 +12496,7 @@
       </c>
       <c r="I38" s="17"/>
     </row>
-    <row r="39" spans="1:9" ht="15.75">
+    <row r="39" spans="1:9" ht="15">
       <c r="A39" s="17"/>
       <c r="B39" s="17" t="s">
         <v>21</v>
@@ -11874,7 +12519,7 @@
       </c>
       <c r="I39" s="17"/>
     </row>
-    <row r="40" spans="1:9" ht="15.75">
+    <row r="40" spans="1:9" ht="15">
       <c r="A40" s="17"/>
       <c r="B40" s="17" t="s">
         <v>21</v>
@@ -11897,7 +12542,7 @@
       </c>
       <c r="I40" s="17"/>
     </row>
-    <row r="41" spans="1:9" ht="15.75">
+    <row r="41" spans="1:9" ht="15">
       <c r="A41" s="17" t="b">
         <v>0</v>
       </c>
@@ -11916,7 +12561,7 @@
       <c r="H41" s="17"/>
       <c r="I41" s="17"/>
     </row>
-    <row r="42" spans="1:9" ht="15.75">
+    <row r="42" spans="1:9" ht="15">
       <c r="A42" s="17"/>
       <c r="B42" s="17" t="s">
         <v>21</v>
@@ -11937,7 +12582,7 @@
       <c r="H42" s="17"/>
       <c r="I42" s="17"/>
     </row>
-    <row r="43" spans="1:9" ht="15.75">
+    <row r="43" spans="1:9" ht="15">
       <c r="A43" s="17"/>
       <c r="B43" s="17" t="s">
         <v>21</v>
@@ -11960,7 +12605,7 @@
       </c>
       <c r="I43" s="17"/>
     </row>
-    <row r="44" spans="1:9" ht="15.75">
+    <row r="44" spans="1:9" ht="15">
       <c r="A44" s="17"/>
       <c r="B44" s="17" t="s">
         <v>21</v>
@@ -11983,7 +12628,7 @@
       </c>
       <c r="I44" s="17"/>
     </row>
-    <row r="45" spans="1:9" ht="15.75">
+    <row r="45" spans="1:9" ht="15">
       <c r="A45" s="17"/>
       <c r="B45" s="17" t="s">
         <v>21</v>
@@ -12006,7 +12651,7 @@
       </c>
       <c r="I45" s="17"/>
     </row>
-    <row r="46" spans="1:9" ht="15.75">
+    <row r="46" spans="1:9" ht="15">
       <c r="A46" s="17"/>
       <c r="B46" s="17" t="s">
         <v>21</v>
@@ -12029,7 +12674,7 @@
       </c>
       <c r="I46" s="17"/>
     </row>
-    <row r="47" spans="1:9" ht="15.75">
+    <row r="47" spans="1:9" ht="15">
       <c r="A47" s="17"/>
       <c r="B47" s="17" t="s">
         <v>21</v>
@@ -12052,7 +12697,7 @@
       </c>
       <c r="I47" s="17"/>
     </row>
-    <row r="48" spans="1:9" ht="15.75">
+    <row r="48" spans="1:9" ht="15">
       <c r="A48" s="17"/>
       <c r="B48" s="17" t="s">
         <v>21</v>
@@ -12075,7 +12720,7 @@
       </c>
       <c r="I48" s="17"/>
     </row>
-    <row r="49" spans="1:9" ht="15.75">
+    <row r="49" spans="1:9" ht="15">
       <c r="A49" s="17"/>
       <c r="B49" s="17" t="s">
         <v>21</v>
@@ -12098,7 +12743,7 @@
       </c>
       <c r="I49" s="17"/>
     </row>
-    <row r="50" spans="1:9" ht="15.75">
+    <row r="50" spans="1:9" ht="15">
       <c r="A50" s="17"/>
       <c r="B50" s="17" t="s">
         <v>21</v>
@@ -12121,7 +12766,7 @@
       </c>
       <c r="I50" s="17"/>
     </row>
-    <row r="51" spans="1:9" ht="15.75">
+    <row r="51" spans="1:9" ht="15">
       <c r="A51" s="17" t="b">
         <v>0</v>
       </c>
@@ -12140,7 +12785,7 @@
       <c r="H51" s="17"/>
       <c r="I51" s="17"/>
     </row>
-    <row r="52" spans="1:9" ht="15.75">
+    <row r="52" spans="1:9" ht="15">
       <c r="A52" s="17"/>
       <c r="B52" s="17" t="s">
         <v>21</v>
@@ -12161,7 +12806,7 @@
       <c r="H52" s="17"/>
       <c r="I52" s="17"/>
     </row>
-    <row r="53" spans="1:9" ht="15.75">
+    <row r="53" spans="1:9" ht="15">
       <c r="A53" s="17"/>
       <c r="B53" s="17" t="s">
         <v>21</v>
@@ -12184,7 +12829,7 @@
       </c>
       <c r="I53" s="17"/>
     </row>
-    <row r="54" spans="1:9" ht="15.75">
+    <row r="54" spans="1:9" ht="15">
       <c r="A54" s="17"/>
       <c r="B54" s="17" t="s">
         <v>21</v>
@@ -12207,7 +12852,7 @@
       </c>
       <c r="I54" s="17"/>
     </row>
-    <row r="55" spans="1:9" ht="15.75">
+    <row r="55" spans="1:9" ht="15">
       <c r="A55" s="17"/>
       <c r="B55" s="17" t="s">
         <v>21</v>
@@ -12230,7 +12875,7 @@
       </c>
       <c r="I55" s="17"/>
     </row>
-    <row r="56" spans="1:9" ht="15.75">
+    <row r="56" spans="1:9" ht="15">
       <c r="A56" s="17"/>
       <c r="B56" s="17" t="s">
         <v>21</v>
@@ -12253,7 +12898,7 @@
       </c>
       <c r="I56" s="17"/>
     </row>
-    <row r="57" spans="1:9" ht="15.75">
+    <row r="57" spans="1:9" ht="15">
       <c r="A57" s="17"/>
       <c r="B57" s="17" t="s">
         <v>21</v>
@@ -12276,7 +12921,7 @@
       </c>
       <c r="I57" s="17"/>
     </row>
-    <row r="58" spans="1:9" ht="15.75">
+    <row r="58" spans="1:9" ht="15">
       <c r="A58" s="17"/>
       <c r="B58" s="17" t="s">
         <v>21</v>
@@ -12299,7 +12944,7 @@
       </c>
       <c r="I58" s="17"/>
     </row>
-    <row r="59" spans="1:9" ht="15.75">
+    <row r="59" spans="1:9" ht="15">
       <c r="A59" s="17"/>
       <c r="B59" s="17" t="s">
         <v>21</v>
@@ -12322,7 +12967,7 @@
       </c>
       <c r="I59" s="17"/>
     </row>
-    <row r="60" spans="1:9" ht="15.75">
+    <row r="60" spans="1:9" ht="15">
       <c r="A60" s="17"/>
       <c r="B60" s="17" t="s">
         <v>21</v>
@@ -12345,7 +12990,7 @@
       </c>
       <c r="I60" s="17"/>
     </row>
-    <row r="61" spans="1:9" ht="15.75">
+    <row r="61" spans="1:9" ht="15">
       <c r="A61" s="17" t="b">
         <v>0</v>
       </c>
@@ -12364,7 +13009,7 @@
       <c r="H61" s="17"/>
       <c r="I61" s="17"/>
     </row>
-    <row r="62" spans="1:9" ht="15.75">
+    <row r="62" spans="1:9" ht="15">
       <c r="A62" s="17"/>
       <c r="B62" s="17" t="s">
         <v>21</v>
@@ -12385,7 +13030,7 @@
       <c r="H62" s="17"/>
       <c r="I62" s="17"/>
     </row>
-    <row r="63" spans="1:9" ht="15.75">
+    <row r="63" spans="1:9" ht="15">
       <c r="A63" s="17"/>
       <c r="B63" s="17" t="s">
         <v>21</v>
@@ -12410,7 +13055,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="15.75">
+    <row r="64" spans="1:9" ht="15">
       <c r="A64" s="17"/>
       <c r="B64" s="17" t="s">
         <v>21</v>
@@ -12433,7 +13078,7 @@
       </c>
       <c r="I64" s="17"/>
     </row>
-    <row r="65" spans="1:9" ht="15.75">
+    <row r="65" spans="1:9" ht="15">
       <c r="A65" s="17"/>
       <c r="B65" s="17" t="s">
         <v>21</v>
@@ -12456,7 +13101,7 @@
       </c>
       <c r="I65" s="17"/>
     </row>
-    <row r="66" spans="1:9" ht="15.75">
+    <row r="66" spans="1:9" ht="15">
       <c r="A66" s="17"/>
       <c r="B66" s="17" t="s">
         <v>21</v>
@@ -12479,7 +13124,7 @@
       </c>
       <c r="I66" s="17"/>
     </row>
-    <row r="67" spans="1:9" ht="15.75">
+    <row r="67" spans="1:9" ht="15">
       <c r="A67" s="17"/>
       <c r="B67" s="17" t="s">
         <v>21</v>
@@ -12502,7 +13147,7 @@
       </c>
       <c r="I67" s="17"/>
     </row>
-    <row r="68" spans="1:9" ht="15.75">
+    <row r="68" spans="1:9" ht="15">
       <c r="A68" s="17"/>
       <c r="B68" s="17" t="s">
         <v>21</v>
@@ -12525,7 +13170,7 @@
       </c>
       <c r="I68" s="17"/>
     </row>
-    <row r="69" spans="1:9" ht="15.75">
+    <row r="69" spans="1:9" ht="15">
       <c r="A69" s="17"/>
       <c r="B69" s="17" t="s">
         <v>21</v>
@@ -12548,7 +13193,7 @@
       </c>
       <c r="I69" s="17"/>
     </row>
-    <row r="70" spans="1:9" ht="15.75">
+    <row r="70" spans="1:9" ht="15">
       <c r="A70" s="17"/>
       <c r="B70" s="17" t="s">
         <v>21</v>
@@ -12571,7 +13216,7 @@
       </c>
       <c r="I70" s="17"/>
     </row>
-    <row r="71" spans="1:9" ht="15.75">
+    <row r="71" spans="1:9" ht="15">
       <c r="A71" s="17"/>
       <c r="B71" s="17" t="s">
         <v>21</v>
@@ -12594,7 +13239,7 @@
       </c>
       <c r="I71" s="17"/>
     </row>
-    <row r="72" spans="1:9" ht="15.75">
+    <row r="72" spans="1:9" ht="15">
       <c r="A72" s="17" t="b">
         <v>0</v>
       </c>
@@ -12613,7 +13258,7 @@
       <c r="H72" s="17"/>
       <c r="I72" s="17"/>
     </row>
-    <row r="73" spans="1:9" ht="15.75">
+    <row r="73" spans="1:9" ht="15">
       <c r="A73" s="17"/>
       <c r="B73" s="17" t="s">
         <v>21</v>
@@ -12634,7 +13279,7 @@
       <c r="H73" s="17"/>
       <c r="I73" s="17"/>
     </row>
-    <row r="74" spans="1:9" ht="15.75">
+    <row r="74" spans="1:9" ht="15">
       <c r="A74" s="17"/>
       <c r="B74" s="17" t="s">
         <v>21</v>
@@ -12657,7 +13302,7 @@
       </c>
       <c r="I74" s="17"/>
     </row>
-    <row r="75" spans="1:9" ht="15.75">
+    <row r="75" spans="1:9" ht="15">
       <c r="A75" s="17"/>
       <c r="B75" s="17" t="s">
         <v>21</v>
@@ -12682,7 +13327,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="15.75">
+    <row r="76" spans="1:9" ht="15">
       <c r="A76" s="17"/>
       <c r="B76" s="17" t="s">
         <v>21</v>
@@ -12705,7 +13350,7 @@
       </c>
       <c r="I76" s="17"/>
     </row>
-    <row r="77" spans="1:9" ht="15.75">
+    <row r="77" spans="1:9" ht="15">
       <c r="A77" s="17"/>
       <c r="B77" s="17" t="s">
         <v>21</v>
@@ -12728,7 +13373,7 @@
       </c>
       <c r="I77" s="17"/>
     </row>
-    <row r="78" spans="1:9" ht="15.75">
+    <row r="78" spans="1:9" ht="15">
       <c r="A78" s="17"/>
       <c r="B78" s="17" t="s">
         <v>21</v>
@@ -12751,7 +13396,7 @@
       </c>
       <c r="I78" s="17"/>
     </row>
-    <row r="79" spans="1:9" ht="15.75">
+    <row r="79" spans="1:9" ht="15">
       <c r="A79" s="17"/>
       <c r="B79" s="17" t="s">
         <v>21</v>
@@ -12774,7 +13419,7 @@
       </c>
       <c r="I79" s="17"/>
     </row>
-    <row r="80" spans="1:9" ht="15.75">
+    <row r="80" spans="1:9" ht="15">
       <c r="A80" s="17"/>
       <c r="B80" s="17" t="s">
         <v>21</v>
@@ -12797,7 +13442,7 @@
       </c>
       <c r="I80" s="17"/>
     </row>
-    <row r="81" spans="1:9" ht="15.75">
+    <row r="81" spans="1:9" ht="15">
       <c r="A81" s="17"/>
       <c r="B81" s="17" t="s">
         <v>21</v>
@@ -12820,7 +13465,7 @@
       </c>
       <c r="I81" s="17"/>
     </row>
-    <row r="82" spans="1:9" ht="15.75">
+    <row r="82" spans="1:9" ht="15">
       <c r="A82" s="17"/>
       <c r="B82" s="17" t="s">
         <v>21</v>
@@ -12843,7 +13488,7 @@
       </c>
       <c r="I82" s="17"/>
     </row>
-    <row r="83" spans="1:9" ht="15.75">
+    <row r="83" spans="1:9" ht="15">
       <c r="A83" s="17"/>
       <c r="B83" s="17" t="s">
         <v>21</v>
@@ -12866,7 +13511,7 @@
       </c>
       <c r="I83" s="17"/>
     </row>
-    <row r="84" spans="1:9" ht="15.75">
+    <row r="84" spans="1:9" ht="15">
       <c r="A84" s="17"/>
       <c r="B84" s="17" t="s">
         <v>21</v>
@@ -12889,7 +13534,7 @@
       </c>
       <c r="I84" s="17"/>
     </row>
-    <row r="85" spans="1:9" ht="15.75">
+    <row r="85" spans="1:9" ht="15">
       <c r="A85" s="17"/>
       <c r="B85" s="17" t="s">
         <v>21</v>
@@ -12912,7 +13557,7 @@
       </c>
       <c r="I85" s="17"/>
     </row>
-    <row r="86" spans="1:9" ht="15.75">
+    <row r="86" spans="1:9" ht="15">
       <c r="A86" s="17" t="b">
         <v>0</v>
       </c>
@@ -12931,7 +13576,7 @@
       <c r="H86" s="17"/>
       <c r="I86" s="17"/>
     </row>
-    <row r="87" spans="1:9" ht="15.75">
+    <row r="87" spans="1:9" ht="15">
       <c r="A87" s="17"/>
       <c r="B87" s="17" t="s">
         <v>21</v>
@@ -12954,7 +13599,7 @@
       </c>
       <c r="I87" s="17"/>
     </row>
-    <row r="88" spans="1:9" ht="15.75">
+    <row r="88" spans="1:9" ht="15">
       <c r="A88" s="17"/>
       <c r="B88" s="17" t="s">
         <v>21</v>
@@ -12977,7 +13622,7 @@
       </c>
       <c r="I88" s="17"/>
     </row>
-    <row r="89" spans="1:9" ht="15.75">
+    <row r="89" spans="1:9" ht="15">
       <c r="A89" s="17"/>
       <c r="B89" s="17" t="s">
         <v>21</v>
@@ -13000,7 +13645,7 @@
       </c>
       <c r="I89" s="17"/>
     </row>
-    <row r="90" spans="1:9" ht="15.75">
+    <row r="90" spans="1:9" ht="15">
       <c r="A90" s="17"/>
       <c r="B90" s="17" t="s">
         <v>21</v>
@@ -13023,7 +13668,7 @@
       </c>
       <c r="I90" s="17"/>
     </row>
-    <row r="91" spans="1:9" ht="15.75">
+    <row r="91" spans="1:9" ht="15">
       <c r="A91" s="17"/>
       <c r="B91" s="17" t="s">
         <v>21</v>
@@ -13046,7 +13691,7 @@
       </c>
       <c r="I91" s="17"/>
     </row>
-    <row r="92" spans="1:9" ht="15.75">
+    <row r="92" spans="1:9" ht="15">
       <c r="A92" s="17"/>
       <c r="B92" s="17" t="s">
         <v>21</v>
@@ -13069,7 +13714,7 @@
       </c>
       <c r="I92" s="17"/>
     </row>
-    <row r="93" spans="1:9" ht="15.75">
+    <row r="93" spans="1:9" ht="15">
       <c r="A93" s="17"/>
       <c r="B93" s="17" t="s">
         <v>21</v>
@@ -13092,7 +13737,7 @@
       </c>
       <c r="I93" s="17"/>
     </row>
-    <row r="94" spans="1:9" ht="15.75">
+    <row r="94" spans="1:9" ht="15">
       <c r="A94" s="17"/>
       <c r="B94" s="17" t="s">
         <v>21</v>
@@ -13115,7 +13760,7 @@
       </c>
       <c r="I94" s="17"/>
     </row>
-    <row r="95" spans="1:9" ht="15.75">
+    <row r="95" spans="1:9" ht="15">
       <c r="A95" s="17"/>
       <c r="B95" s="17" t="s">
         <v>21</v>
@@ -13138,7 +13783,7 @@
       </c>
       <c r="I95" s="17"/>
     </row>
-    <row r="96" spans="1:9" ht="15.75">
+    <row r="96" spans="1:9" ht="15">
       <c r="A96" s="17"/>
       <c r="B96" s="17" t="s">
         <v>21</v>
@@ -13161,7 +13806,7 @@
       </c>
       <c r="I96" s="17"/>
     </row>
-    <row r="97" spans="1:9" ht="15.75">
+    <row r="97" spans="1:9" ht="15">
       <c r="A97" s="17" t="b">
         <v>0</v>
       </c>
@@ -13180,7 +13825,7 @@
       <c r="H97" s="17"/>
       <c r="I97" s="17"/>
     </row>
-    <row r="98" spans="1:9" ht="15.75">
+    <row r="98" spans="1:9" ht="15">
       <c r="A98" s="17"/>
       <c r="B98" s="17" t="s">
         <v>21</v>
@@ -13205,7 +13850,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="15.75">
+    <row r="99" spans="1:9" ht="15">
       <c r="A99" s="17" t="b">
         <v>0</v>
       </c>
@@ -13224,7 +13869,7 @@
       <c r="H99" s="17"/>
       <c r="I99" s="17"/>
     </row>
-    <row r="100" spans="1:9" ht="15.75">
+    <row r="100" spans="1:9" ht="15">
       <c r="A100" s="17"/>
       <c r="B100" s="17" t="s">
         <v>21</v>
@@ -13245,7 +13890,7 @@
       <c r="H100" s="17"/>
       <c r="I100" s="17"/>
     </row>
-    <row r="101" spans="1:9" ht="15.75">
+    <row r="101" spans="1:9" ht="15">
       <c r="A101" s="17"/>
       <c r="B101" s="17" t="s">
         <v>21</v>
@@ -13270,7 +13915,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="15.75">
+    <row r="102" spans="1:9" ht="15">
       <c r="A102" s="17" t="b">
         <v>0</v>
       </c>
@@ -13289,7 +13934,7 @@
       <c r="H102" s="17"/>
       <c r="I102" s="17"/>
     </row>
-    <row r="103" spans="1:9" ht="15.75">
+    <row r="103" spans="1:9" ht="15">
       <c r="A103" s="17"/>
       <c r="B103" s="17" t="s">
         <v>21</v>
@@ -13312,7 +13957,7 @@
       </c>
       <c r="I103" s="17"/>
     </row>
-    <row r="104" spans="1:9" ht="15.75">
+    <row r="104" spans="1:9" ht="15">
       <c r="A104" s="17"/>
       <c r="B104" s="17" t="s">
         <v>21</v>
@@ -13337,7 +13982,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="15.75">
+    <row r="105" spans="1:9" ht="15">
       <c r="A105" s="17"/>
       <c r="B105" s="17" t="s">
         <v>21</v>
@@ -13360,7 +14005,7 @@
       </c>
       <c r="I105" s="17"/>
     </row>
-    <row r="106" spans="1:9" ht="15.75">
+    <row r="106" spans="1:9" ht="15">
       <c r="A106" s="17"/>
       <c r="B106" s="17" t="s">
         <v>21</v>
@@ -13381,7 +14026,7 @@
       <c r="H106" s="17"/>
       <c r="I106" s="17"/>
     </row>
-    <row r="107" spans="1:9" ht="15.75">
+    <row r="107" spans="1:9" ht="15">
       <c r="A107" s="17" t="b">
         <v>0</v>
       </c>
@@ -13400,7 +14045,7 @@
       <c r="H107" s="17"/>
       <c r="I107" s="17"/>
     </row>
-    <row r="108" spans="1:9" ht="15.75">
+    <row r="108" spans="1:9" ht="15">
       <c r="A108" s="17"/>
       <c r="B108" s="17" t="s">
         <v>21</v>
@@ -13425,7 +14070,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="15.75">
+    <row r="109" spans="1:9" ht="15">
       <c r="A109" s="17"/>
       <c r="B109" s="17" t="s">
         <v>21</v>
@@ -13448,7 +14093,7 @@
       </c>
       <c r="I109" s="17"/>
     </row>
-    <row r="110" spans="1:9" ht="15.75">
+    <row r="110" spans="1:9" ht="15">
       <c r="A110" s="17"/>
       <c r="B110" s="17" t="s">
         <v>21</v>
@@ -13471,7 +14116,7 @@
       </c>
       <c r="I110" s="17"/>
     </row>
-    <row r="111" spans="1:9" ht="15.75">
+    <row r="111" spans="1:9" ht="15">
       <c r="A111" s="17"/>
       <c r="B111" s="17" t="s">
         <v>21</v>
@@ -13494,7 +14139,7 @@
       </c>
       <c r="I111" s="17"/>
     </row>
-    <row r="112" spans="1:9" ht="15.75">
+    <row r="112" spans="1:9" ht="15">
       <c r="A112" s="17"/>
       <c r="B112" s="17" t="s">
         <v>21</v>
@@ -13517,7 +14162,7 @@
       </c>
       <c r="I112" s="17"/>
     </row>
-    <row r="113" spans="1:9" ht="15.75">
+    <row r="113" spans="1:9" ht="15">
       <c r="A113" s="17"/>
       <c r="B113" s="17" t="s">
         <v>21</v>
@@ -13540,7 +14185,7 @@
       </c>
       <c r="I113" s="17"/>
     </row>
-    <row r="114" spans="1:9" ht="15.75">
+    <row r="114" spans="1:9" ht="15">
       <c r="A114" s="17"/>
       <c r="B114" s="17" t="s">
         <v>21</v>
@@ -13563,7 +14208,7 @@
       </c>
       <c r="I114" s="17"/>
     </row>
-    <row r="115" spans="1:9" ht="15.75">
+    <row r="115" spans="1:9" ht="15">
       <c r="A115" s="17" t="b">
         <v>0</v>
       </c>
@@ -13582,7 +14227,7 @@
       <c r="H115" s="17"/>
       <c r="I115" s="17"/>
     </row>
-    <row r="116" spans="1:9" ht="15.75">
+    <row r="116" spans="1:9" ht="15">
       <c r="A116" s="17"/>
       <c r="B116" s="17" t="s">
         <v>21</v>
@@ -13605,7 +14250,7 @@
       </c>
       <c r="I116" s="17"/>
     </row>
-    <row r="117" spans="1:9" ht="15.75">
+    <row r="117" spans="1:9" ht="15">
       <c r="A117" s="17"/>
       <c r="B117" s="17" t="s">
         <v>21</v>
@@ -13628,7 +14273,7 @@
       </c>
       <c r="I117" s="17"/>
     </row>
-    <row r="118" spans="1:9" ht="15.75">
+    <row r="118" spans="1:9" ht="15">
       <c r="A118" s="17"/>
       <c r="B118" s="17" t="s">
         <v>21</v>
@@ -13651,7 +14296,7 @@
       </c>
       <c r="I118" s="17"/>
     </row>
-    <row r="119" spans="1:9" ht="15.75">
+    <row r="119" spans="1:9" ht="15">
       <c r="A119" s="17" t="b">
         <v>0</v>
       </c>
@@ -13670,7 +14315,7 @@
       <c r="H119" s="17"/>
       <c r="I119" s="17"/>
     </row>
-    <row r="120" spans="1:9" ht="15.75">
+    <row r="120" spans="1:9" ht="15">
       <c r="A120" s="17"/>
       <c r="B120" s="17" t="s">
         <v>21</v>
@@ -13693,7 +14338,7 @@
       </c>
       <c r="I120" s="17"/>
     </row>
-    <row r="121" spans="1:9" ht="15.75">
+    <row r="121" spans="1:9" ht="15">
       <c r="A121" s="17"/>
       <c r="B121" s="17" t="s">
         <v>21</v>
@@ -13716,7 +14361,7 @@
       </c>
       <c r="I121" s="17"/>
     </row>
-    <row r="122" spans="1:9" ht="15.75">
+    <row r="122" spans="1:9" ht="15">
       <c r="A122" s="17"/>
       <c r="B122" s="17" t="s">
         <v>21</v>
@@ -13739,7 +14384,7 @@
       </c>
       <c r="I122" s="17"/>
     </row>
-    <row r="123" spans="1:9" ht="15.75">
+    <row r="123" spans="1:9" ht="15">
       <c r="A123" s="17"/>
       <c r="B123" s="17" t="s">
         <v>21</v>
@@ -13762,7 +14407,7 @@
       </c>
       <c r="I123" s="17"/>
     </row>
-    <row r="124" spans="1:9" ht="15.75">
+    <row r="124" spans="1:9" ht="15">
       <c r="A124" s="17"/>
       <c r="B124" s="17" t="s">
         <v>21</v>
@@ -13785,7 +14430,7 @@
       </c>
       <c r="I124" s="17"/>
     </row>
-    <row r="125" spans="1:9" ht="15.75">
+    <row r="125" spans="1:9" ht="15">
       <c r="A125" s="17"/>
       <c r="B125" s="17" t="s">
         <v>21</v>
@@ -13808,7 +14453,7 @@
       </c>
       <c r="I125" s="17"/>
     </row>
-    <row r="126" spans="1:9" ht="15.75">
+    <row r="126" spans="1:9" ht="15">
       <c r="A126" s="17" t="b">
         <v>0</v>
       </c>
@@ -13827,7 +14472,7 @@
       <c r="H126" s="17"/>
       <c r="I126" s="17"/>
     </row>
-    <row r="127" spans="1:9" ht="15.75">
+    <row r="127" spans="1:9" ht="15">
       <c r="A127" s="17"/>
       <c r="B127" s="17" t="s">
         <v>21</v>
@@ -13852,7 +14497,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="15.75">
+    <row r="128" spans="1:9" ht="15">
       <c r="A128" s="17"/>
       <c r="B128" s="17" t="s">
         <v>21</v>
@@ -13875,7 +14520,7 @@
       </c>
       <c r="I128" s="17"/>
     </row>
-    <row r="129" spans="1:9" ht="15.75">
+    <row r="129" spans="1:9" ht="15">
       <c r="A129" s="17"/>
       <c r="B129" s="17" t="s">
         <v>21</v>
@@ -13898,7 +14543,7 @@
       </c>
       <c r="I129" s="17"/>
     </row>
-    <row r="130" spans="1:9" ht="15.75">
+    <row r="130" spans="1:9" ht="15">
       <c r="A130" s="17"/>
       <c r="B130" s="17" t="s">
         <v>21</v>
@@ -13921,7 +14566,7 @@
       </c>
       <c r="I130" s="17"/>
     </row>
-    <row r="131" spans="1:9" ht="15.75">
+    <row r="131" spans="1:9" ht="15">
       <c r="A131" s="17"/>
       <c r="B131" s="17" t="s">
         <v>21</v>
@@ -13944,7 +14589,7 @@
       </c>
       <c r="I131" s="17"/>
     </row>
-    <row r="132" spans="1:9" ht="15.75">
+    <row r="132" spans="1:9" ht="15">
       <c r="A132" s="17"/>
       <c r="B132" s="17" t="s">
         <v>21</v>
@@ -13967,7 +14612,7 @@
       </c>
       <c r="I132" s="17"/>
     </row>
-    <row r="133" spans="1:9" ht="15.75">
+    <row r="133" spans="1:9" ht="15">
       <c r="A133" s="17"/>
       <c r="B133" s="17" t="s">
         <v>21</v>
@@ -13990,7 +14635,7 @@
       </c>
       <c r="I133" s="17"/>
     </row>
-    <row r="134" spans="1:9" ht="15.75">
+    <row r="134" spans="1:9" ht="15">
       <c r="A134" s="17"/>
       <c r="B134" s="17" t="s">
         <v>21</v>
@@ -14013,7 +14658,7 @@
       </c>
       <c r="I134" s="17"/>
     </row>
-    <row r="135" spans="1:9" ht="15.75">
+    <row r="135" spans="1:9" ht="15">
       <c r="A135" s="17"/>
       <c r="B135" s="17" t="s">
         <v>21</v>
@@ -14036,7 +14681,7 @@
       </c>
       <c r="I135" s="17"/>
     </row>
-    <row r="136" spans="1:9" ht="15.75">
+    <row r="136" spans="1:9" ht="15">
       <c r="A136" s="17" t="b">
         <v>0</v>
       </c>
@@ -14055,7 +14700,7 @@
       <c r="H136" s="17"/>
       <c r="I136" s="17"/>
     </row>
-    <row r="137" spans="1:9" ht="15.75">
+    <row r="137" spans="1:9" ht="15">
       <c r="A137" s="17"/>
       <c r="B137" s="17" t="s">
         <v>21</v>
@@ -14080,7 +14725,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="15.75">
+    <row r="138" spans="1:9" ht="15">
       <c r="A138" s="17"/>
       <c r="B138" s="17" t="s">
         <v>21</v>
@@ -14101,7 +14746,7 @@
       <c r="H138" s="17"/>
       <c r="I138" s="17"/>
     </row>
-    <row r="139" spans="1:9" ht="15.75">
+    <row r="139" spans="1:9" ht="15">
       <c r="A139" s="17"/>
       <c r="B139" s="17" t="s">
         <v>21</v>
@@ -14124,7 +14769,7 @@
       </c>
       <c r="I139" s="17"/>
     </row>
-    <row r="140" spans="1:9" ht="15.75">
+    <row r="140" spans="1:9" ht="15">
       <c r="A140" s="17"/>
       <c r="B140" s="17" t="s">
         <v>21</v>
@@ -14147,7 +14792,7 @@
       </c>
       <c r="I140" s="17"/>
     </row>
-    <row r="141" spans="1:9" ht="15.75">
+    <row r="141" spans="1:9" ht="15">
       <c r="A141" s="17"/>
       <c r="B141" s="17" t="s">
         <v>21</v>
@@ -14170,7 +14815,7 @@
       </c>
       <c r="I141" s="17"/>
     </row>
-    <row r="142" spans="1:9" ht="15.75">
+    <row r="142" spans="1:9" ht="15">
       <c r="A142" s="17"/>
       <c r="B142" s="17" t="s">
         <v>21</v>
@@ -14193,7 +14838,7 @@
       </c>
       <c r="I142" s="17"/>
     </row>
-    <row r="143" spans="1:9" ht="15.75">
+    <row r="143" spans="1:9" ht="15">
       <c r="A143" s="17"/>
       <c r="B143" s="17" t="s">
         <v>21</v>
@@ -14216,7 +14861,7 @@
       </c>
       <c r="I143" s="17"/>
     </row>
-    <row r="144" spans="1:9" ht="15.75">
+    <row r="144" spans="1:9" ht="15">
       <c r="A144" s="17"/>
       <c r="B144" s="17" t="s">
         <v>21</v>
@@ -14239,7 +14884,7 @@
       </c>
       <c r="I144" s="17"/>
     </row>
-    <row r="145" spans="1:9" ht="15.75">
+    <row r="145" spans="1:9" ht="15">
       <c r="A145" s="17"/>
       <c r="B145" s="17" t="s">
         <v>21</v>
@@ -14262,7 +14907,7 @@
       </c>
       <c r="I145" s="17"/>
     </row>
-    <row r="146" spans="1:9" ht="15.75">
+    <row r="146" spans="1:9" ht="15">
       <c r="A146" s="17"/>
       <c r="B146" s="17" t="s">
         <v>21</v>
@@ -14285,7 +14930,7 @@
       </c>
       <c r="I146" s="17"/>
     </row>
-    <row r="147" spans="1:9" ht="15.75">
+    <row r="147" spans="1:9" ht="15">
       <c r="A147" s="17"/>
       <c r="B147" s="17" t="s">
         <v>21</v>
@@ -14308,7 +14953,7 @@
       </c>
       <c r="I147" s="17"/>
     </row>
-    <row r="148" spans="1:9" ht="15.75">
+    <row r="148" spans="1:9" ht="15">
       <c r="A148" s="17"/>
       <c r="B148" s="17" t="s">
         <v>21</v>
@@ -14331,7 +14976,7 @@
       </c>
       <c r="I148" s="17"/>
     </row>
-    <row r="149" spans="1:9" ht="15.75">
+    <row r="149" spans="1:9" ht="15">
       <c r="A149" s="17"/>
       <c r="B149" s="17" t="s">
         <v>21</v>
@@ -14354,7 +14999,7 @@
       </c>
       <c r="I149" s="17"/>
     </row>
-    <row r="150" spans="1:9" ht="15.75">
+    <row r="150" spans="1:9" ht="15">
       <c r="A150" s="17"/>
       <c r="B150" s="17" t="s">
         <v>21</v>
@@ -14377,7 +15022,7 @@
       </c>
       <c r="I150" s="17"/>
     </row>
-    <row r="151" spans="1:9" ht="15.75">
+    <row r="151" spans="1:9" ht="15">
       <c r="A151" s="17" t="b">
         <v>0</v>
       </c>
@@ -14396,7 +15041,7 @@
       <c r="H151" s="17"/>
       <c r="I151" s="17"/>
     </row>
-    <row r="152" spans="1:9" ht="15.75">
+    <row r="152" spans="1:9" ht="15">
       <c r="A152" s="17"/>
       <c r="B152" s="17" t="s">
         <v>21</v>
@@ -14419,7 +15064,7 @@
       </c>
       <c r="I152" s="17"/>
     </row>
-    <row r="153" spans="1:9" ht="15.75">
+    <row r="153" spans="1:9" ht="15">
       <c r="A153" s="17" t="b">
         <v>0</v>
       </c>
@@ -14438,7 +15083,7 @@
       <c r="H153" s="17"/>
       <c r="I153" s="17"/>
     </row>
-    <row r="154" spans="1:9" ht="15.75">
+    <row r="154" spans="1:9" ht="15">
       <c r="A154" s="17"/>
       <c r="B154" s="17" t="s">
         <v>21</v>
@@ -14461,7 +15106,7 @@
       </c>
       <c r="I154" s="17"/>
     </row>
-    <row r="155" spans="1:9" ht="15.75">
+    <row r="155" spans="1:9" ht="15">
       <c r="A155" s="17"/>
       <c r="B155" s="17" t="s">
         <v>21</v>
@@ -14484,7 +15129,7 @@
       </c>
       <c r="I155" s="17"/>
     </row>
-    <row r="156" spans="1:9" ht="15.75">
+    <row r="156" spans="1:9" ht="15">
       <c r="A156" s="17" t="b">
         <v>0</v>
       </c>
@@ -14503,7 +15148,7 @@
       <c r="H156" s="17"/>
       <c r="I156" s="17"/>
     </row>
-    <row r="157" spans="1:9" ht="15.75">
+    <row r="157" spans="1:9" ht="15">
       <c r="A157" s="17"/>
       <c r="B157" s="17" t="s">
         <v>21</v>
@@ -14528,7 +15173,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="158" spans="1:9" ht="15.75">
+    <row r="158" spans="1:9" ht="15">
       <c r="A158" s="17"/>
       <c r="B158" s="17" t="s">
         <v>21</v>
@@ -14551,7 +15196,7 @@
       </c>
       <c r="I158" s="17"/>
     </row>
-    <row r="159" spans="1:9" ht="15.75">
+    <row r="159" spans="1:9" ht="15">
       <c r="A159" s="17"/>
       <c r="B159" s="17" t="s">
         <v>21</v>
@@ -14574,7 +15219,7 @@
       </c>
       <c r="I159" s="17"/>
     </row>
-    <row r="160" spans="1:9" ht="15.75">
+    <row r="160" spans="1:9" ht="15">
       <c r="A160" s="17"/>
       <c r="B160" s="17" t="s">
         <v>21</v>
@@ -14597,7 +15242,7 @@
       </c>
       <c r="I160" s="17"/>
     </row>
-    <row r="161" spans="1:9" ht="15.75">
+    <row r="161" spans="1:9" ht="15">
       <c r="A161" s="17"/>
       <c r="B161" s="17" t="s">
         <v>21</v>
@@ -14620,7 +15265,7 @@
       </c>
       <c r="I161" s="17"/>
     </row>
-    <row r="162" spans="1:9" ht="15.75">
+    <row r="162" spans="1:9" ht="15">
       <c r="A162" s="17"/>
       <c r="B162" s="17" t="s">
         <v>21</v>
@@ -14643,7 +15288,7 @@
       </c>
       <c r="I162" s="17"/>
     </row>
-    <row r="163" spans="1:9" ht="15.75">
+    <row r="163" spans="1:9" ht="15">
       <c r="A163" s="17"/>
       <c r="B163" s="17" t="s">
         <v>21</v>
@@ -14666,7 +15311,7 @@
       </c>
       <c r="I163" s="17"/>
     </row>
-    <row r="164" spans="1:9" ht="15.75">
+    <row r="164" spans="1:9" ht="15">
       <c r="A164" s="17"/>
       <c r="B164" s="17" t="s">
         <v>21</v>
@@ -14689,7 +15334,7 @@
       </c>
       <c r="I164" s="17"/>
     </row>
-    <row r="165" spans="1:9" ht="15.75">
+    <row r="165" spans="1:9" ht="15">
       <c r="A165" s="17"/>
       <c r="B165" s="17" t="s">
         <v>21</v>
@@ -14712,7 +15357,7 @@
       </c>
       <c r="I165" s="17"/>
     </row>
-    <row r="166" spans="1:9" ht="15.75">
+    <row r="166" spans="1:9" ht="15">
       <c r="A166" s="17"/>
       <c r="B166" s="17" t="s">
         <v>21</v>
@@ -14735,7 +15380,7 @@
       </c>
       <c r="I166" s="17"/>
     </row>
-    <row r="167" spans="1:9" ht="15.75">
+    <row r="167" spans="1:9" ht="15">
       <c r="A167" s="17" t="b">
         <v>0</v>
       </c>
@@ -14754,7 +15399,7 @@
       <c r="H167" s="17"/>
       <c r="I167" s="17"/>
     </row>
-    <row r="168" spans="1:9" ht="15.75">
+    <row r="168" spans="1:9" ht="15">
       <c r="A168" s="17"/>
       <c r="B168" s="17" t="s">
         <v>21</v>
@@ -14779,7 +15424,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="169" spans="1:9" ht="15.75">
+    <row r="169" spans="1:9" ht="15">
       <c r="A169" s="17"/>
       <c r="B169" s="17" t="s">
         <v>21</v>
@@ -14802,7 +15447,7 @@
       </c>
       <c r="I169" s="17"/>
     </row>
-    <row r="170" spans="1:9" ht="15.75">
+    <row r="170" spans="1:9" ht="15">
       <c r="A170" s="17"/>
       <c r="B170" s="17" t="s">
         <v>21</v>
@@ -14825,7 +15470,7 @@
       </c>
       <c r="I170" s="17"/>
     </row>
-    <row r="171" spans="1:9" ht="15.75">
+    <row r="171" spans="1:9" ht="15">
       <c r="A171" s="17"/>
       <c r="B171" s="17" t="s">
         <v>21</v>
@@ -14848,7 +15493,7 @@
       </c>
       <c r="I171" s="17"/>
     </row>
-    <row r="172" spans="1:9" ht="15.75">
+    <row r="172" spans="1:9" ht="15">
       <c r="A172" s="17"/>
       <c r="B172" s="17" t="s">
         <v>21</v>
@@ -14871,7 +15516,7 @@
       </c>
       <c r="I172" s="17"/>
     </row>
-    <row r="173" spans="1:9" ht="15.75">
+    <row r="173" spans="1:9" ht="15">
       <c r="A173" s="17"/>
       <c r="B173" s="17" t="s">
         <v>21</v>
@@ -14894,7 +15539,7 @@
       </c>
       <c r="I173" s="17"/>
     </row>
-    <row r="174" spans="1:9" ht="15.75">
+    <row r="174" spans="1:9" ht="15">
       <c r="A174" s="17"/>
       <c r="B174" s="17" t="s">
         <v>21</v>
@@ -14917,7 +15562,7 @@
       </c>
       <c r="I174" s="17"/>
     </row>
-    <row r="175" spans="1:9" ht="15.75">
+    <row r="175" spans="1:9" ht="15">
       <c r="A175" s="17"/>
       <c r="B175" s="17" t="s">
         <v>21</v>
@@ -14940,7 +15585,7 @@
       </c>
       <c r="I175" s="17"/>
     </row>
-    <row r="176" spans="1:9" ht="15.75">
+    <row r="176" spans="1:9" ht="15">
       <c r="A176" s="17"/>
       <c r="B176" s="17" t="s">
         <v>21</v>
@@ -14963,7 +15608,7 @@
       </c>
       <c r="I176" s="17"/>
     </row>
-    <row r="177" spans="1:9" ht="15.75">
+    <row r="177" spans="1:9" ht="15">
       <c r="A177" s="17"/>
       <c r="B177" s="17" t="s">
         <v>21</v>
@@ -14986,7 +15631,7 @@
       </c>
       <c r="I177" s="17"/>
     </row>
-    <row r="178" spans="1:9" ht="15.75">
+    <row r="178" spans="1:9" ht="15">
       <c r="A178" s="17" t="b">
         <v>0</v>
       </c>
@@ -15005,7 +15650,7 @@
       <c r="H178" s="17"/>
       <c r="I178" s="17"/>
     </row>
-    <row r="179" spans="1:9" ht="15.75">
+    <row r="179" spans="1:9" ht="15">
       <c r="A179" s="17"/>
       <c r="B179" s="17" t="s">
         <v>21</v>
@@ -15028,7 +15673,7 @@
       </c>
       <c r="I179" s="17"/>
     </row>
-    <row r="180" spans="1:9" ht="15.75">
+    <row r="180" spans="1:9" ht="15">
       <c r="A180" s="17"/>
       <c r="B180" s="17" t="s">
         <v>21</v>
@@ -15051,7 +15696,7 @@
       </c>
       <c r="I180" s="17"/>
     </row>
-    <row r="181" spans="1:9" ht="15.75">
+    <row r="181" spans="1:9" ht="15">
       <c r="A181" s="17"/>
       <c r="B181" s="17" t="s">
         <v>21</v>
@@ -15074,7 +15719,7 @@
       </c>
       <c r="I181" s="17"/>
     </row>
-    <row r="182" spans="1:9" ht="15.75">
+    <row r="182" spans="1:9" ht="15">
       <c r="A182" s="17"/>
       <c r="B182" s="17" t="s">
         <v>21</v>
@@ -15097,7 +15742,7 @@
       </c>
       <c r="I182" s="17"/>
     </row>
-    <row r="183" spans="1:9" ht="15.75">
+    <row r="183" spans="1:9" ht="15">
       <c r="A183" s="17" t="b">
         <v>0</v>
       </c>
@@ -15116,7 +15761,7 @@
       <c r="H183" s="17"/>
       <c r="I183" s="17"/>
     </row>
-    <row r="184" spans="1:9" ht="15.75">
+    <row r="184" spans="1:9" ht="15">
       <c r="A184" s="17"/>
       <c r="B184" s="17" t="s">
         <v>21</v>
@@ -15139,7 +15784,7 @@
       </c>
       <c r="I184" s="17"/>
     </row>
-    <row r="185" spans="1:9" ht="15.75">
+    <row r="185" spans="1:9" ht="15">
       <c r="A185" s="17"/>
       <c r="B185" s="17" t="s">
         <v>21</v>
@@ -15162,7 +15807,7 @@
       </c>
       <c r="I185" s="17"/>
     </row>
-    <row r="186" spans="1:9" ht="15.75">
+    <row r="186" spans="1:9" ht="15">
       <c r="A186" s="17"/>
       <c r="B186" s="17" t="s">
         <v>21</v>
@@ -15185,7 +15830,7 @@
       </c>
       <c r="I186" s="17"/>
     </row>
-    <row r="187" spans="1:9" ht="15.75">
+    <row r="187" spans="1:9" ht="15">
       <c r="A187" s="17"/>
       <c r="B187" s="17" t="s">
         <v>21</v>
@@ -15208,7 +15853,7 @@
       </c>
       <c r="I187" s="17"/>
     </row>
-    <row r="188" spans="1:9" ht="15.75">
+    <row r="188" spans="1:9" ht="15">
       <c r="A188" s="17" t="b">
         <v>0</v>
       </c>
@@ -15227,7 +15872,7 @@
       <c r="H188" s="17"/>
       <c r="I188" s="17"/>
     </row>
-    <row r="189" spans="1:9" ht="15.75">
+    <row r="189" spans="1:9" ht="15">
       <c r="A189" s="17"/>
       <c r="B189" s="17" t="s">
         <v>21</v>
@@ -15248,7 +15893,7 @@
       <c r="H189" s="17"/>
       <c r="I189" s="17"/>
     </row>
-    <row r="190" spans="1:9" ht="15.75">
+    <row r="190" spans="1:9" ht="15">
       <c r="A190" s="17"/>
       <c r="B190" s="17" t="s">
         <v>21</v>
@@ -15271,7 +15916,7 @@
       </c>
       <c r="I190" s="17"/>
     </row>
-    <row r="191" spans="1:9" ht="15.75">
+    <row r="191" spans="1:9" ht="15">
       <c r="A191" s="17" t="b">
         <v>0</v>
       </c>
@@ -15290,7 +15935,7 @@
       <c r="H191" s="17"/>
       <c r="I191" s="17"/>
     </row>
-    <row r="192" spans="1:9" ht="15.75">
+    <row r="192" spans="1:9" ht="15">
       <c r="A192" s="17"/>
       <c r="B192" s="17" t="s">
         <v>21</v>
@@ -15313,7 +15958,7 @@
       </c>
       <c r="I192" s="17"/>
     </row>
-    <row r="193" spans="1:9" ht="15.75">
+    <row r="193" spans="1:9" ht="15">
       <c r="A193" s="17"/>
       <c r="B193" s="17" t="s">
         <v>21</v>
@@ -15338,7 +15983,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="194" spans="1:9" ht="15.75">
+    <row r="194" spans="1:9" ht="15">
       <c r="A194" s="17"/>
       <c r="B194" s="17" t="s">
         <v>21</v>
@@ -15359,7 +16004,7 @@
       <c r="H194" s="17"/>
       <c r="I194" s="17"/>
     </row>
-    <row r="195" spans="1:9" ht="15.75">
+    <row r="195" spans="1:9" ht="15">
       <c r="A195" s="17"/>
       <c r="B195" s="17" t="s">
         <v>21</v>
@@ -15384,7 +16029,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="196" spans="1:9" ht="15.75">
+    <row r="196" spans="1:9" ht="15">
       <c r="A196" s="17"/>
       <c r="B196" s="17" t="s">
         <v>21</v>
@@ -15409,7 +16054,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="197" spans="1:9" ht="15.75">
+    <row r="197" spans="1:9" ht="15">
       <c r="A197" s="17" t="b">
         <v>0</v>
       </c>
@@ -15428,7 +16073,7 @@
       <c r="H197" s="17"/>
       <c r="I197" s="17"/>
     </row>
-    <row r="198" spans="1:9" ht="15.75">
+    <row r="198" spans="1:9" ht="15">
       <c r="A198" s="17"/>
       <c r="B198" s="17" t="s">
         <v>21</v>
@@ -15453,7 +16098,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="199" spans="1:9" ht="15.75">
+    <row r="199" spans="1:9" ht="15">
       <c r="A199" s="17"/>
       <c r="B199" s="17" t="s">
         <v>21</v>
@@ -15476,7 +16121,7 @@
       </c>
       <c r="I199" s="17"/>
     </row>
-    <row r="200" spans="1:9" ht="15.75">
+    <row r="200" spans="1:9" ht="15">
       <c r="A200" s="17"/>
       <c r="B200" s="17" t="s">
         <v>21</v>
@@ -15499,7 +16144,7 @@
       </c>
       <c r="I200" s="17"/>
     </row>
-    <row r="201" spans="1:9" ht="15.75">
+    <row r="201" spans="1:9" ht="15">
       <c r="A201" s="17"/>
       <c r="B201" s="17" t="s">
         <v>21</v>
@@ -15522,7 +16167,7 @@
       </c>
       <c r="I201" s="17"/>
     </row>
-    <row r="202" spans="1:9" ht="15.75">
+    <row r="202" spans="1:9" ht="15">
       <c r="A202" s="17"/>
       <c r="B202" s="17" t="s">
         <v>21</v>
@@ -15545,7 +16190,7 @@
       </c>
       <c r="I202" s="17"/>
     </row>
-    <row r="203" spans="1:9" ht="15.75">
+    <row r="203" spans="1:9" ht="15">
       <c r="A203" s="17"/>
       <c r="B203" s="17" t="s">
         <v>21</v>
@@ -15568,7 +16213,7 @@
       </c>
       <c r="I203" s="17"/>
     </row>
-    <row r="204" spans="1:9" ht="15.75">
+    <row r="204" spans="1:9" ht="15">
       <c r="A204" s="17"/>
       <c r="B204" s="17" t="s">
         <v>21</v>
@@ -15591,7 +16236,7 @@
       </c>
       <c r="I204" s="17"/>
     </row>
-    <row r="205" spans="1:9" ht="15.75">
+    <row r="205" spans="1:9" ht="15">
       <c r="A205" s="17"/>
       <c r="B205" s="17" t="s">
         <v>21</v>
@@ -15614,7 +16259,7 @@
       </c>
       <c r="I205" s="17"/>
     </row>
-    <row r="206" spans="1:9" ht="15.75">
+    <row r="206" spans="1:9" ht="15">
       <c r="A206" s="17"/>
       <c r="B206" s="17" t="s">
         <v>21</v>
@@ -15637,7 +16282,7 @@
       </c>
       <c r="I206" s="17"/>
     </row>
-    <row r="207" spans="1:9" ht="15.75">
+    <row r="207" spans="1:9" ht="15">
       <c r="A207" s="17" t="b">
         <v>0</v>
       </c>
@@ -15656,7 +16301,7 @@
       <c r="H207" s="17"/>
       <c r="I207" s="17"/>
     </row>
-    <row r="208" spans="1:9" ht="15.75">
+    <row r="208" spans="1:9" ht="15">
       <c r="A208" s="17"/>
       <c r="B208" s="17" t="s">
         <v>21</v>
@@ -15681,7 +16326,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="209" spans="1:9" ht="15.75">
+    <row r="209" spans="1:9" ht="15">
       <c r="A209" s="17"/>
       <c r="B209" s="17" t="s">
         <v>21</v>
@@ -15704,7 +16349,7 @@
       </c>
       <c r="I209" s="17"/>
     </row>
-    <row r="210" spans="1:9" ht="15.75">
+    <row r="210" spans="1:9" ht="15">
       <c r="A210" s="17"/>
       <c r="B210" s="17" t="s">
         <v>21</v>
@@ -15727,7 +16372,7 @@
       </c>
       <c r="I210" s="17"/>
     </row>
-    <row r="211" spans="1:9" ht="15.75">
+    <row r="211" spans="1:9" ht="15">
       <c r="A211" s="17"/>
       <c r="B211" s="17" t="s">
         <v>21</v>
@@ -15750,7 +16395,7 @@
       </c>
       <c r="I211" s="17"/>
     </row>
-    <row r="212" spans="1:9" ht="15.75">
+    <row r="212" spans="1:9" ht="15">
       <c r="A212" s="17"/>
       <c r="B212" s="17" t="s">
         <v>21</v>
@@ -15773,7 +16418,7 @@
       </c>
       <c r="I212" s="17"/>
     </row>
-    <row r="213" spans="1:9" ht="15.75">
+    <row r="213" spans="1:9" ht="15">
       <c r="A213" s="17"/>
       <c r="B213" s="17" t="s">
         <v>21</v>
@@ -15796,7 +16441,7 @@
       </c>
       <c r="I213" s="17"/>
     </row>
-    <row r="214" spans="1:9" ht="15.75">
+    <row r="214" spans="1:9" ht="15">
       <c r="A214" s="17"/>
       <c r="B214" s="17" t="s">
         <v>21</v>
@@ -15819,7 +16464,7 @@
       </c>
       <c r="I214" s="17"/>
     </row>
-    <row r="215" spans="1:9" ht="15.75">
+    <row r="215" spans="1:9" ht="15">
       <c r="A215" s="17"/>
       <c r="B215" s="17" t="s">
         <v>21</v>
@@ -15842,7 +16487,7 @@
       </c>
       <c r="I215" s="17"/>
     </row>
-    <row r="216" spans="1:9" ht="15.75">
+    <row r="216" spans="1:9" ht="15">
       <c r="A216" s="17"/>
       <c r="B216" s="17" t="s">
         <v>21</v>
@@ -15865,7 +16510,7 @@
       </c>
       <c r="I216" s="17"/>
     </row>
-    <row r="217" spans="1:9" ht="15.75">
+    <row r="217" spans="1:9" ht="15">
       <c r="A217" s="17" t="b">
         <v>0</v>
       </c>
@@ -15884,7 +16529,7 @@
       <c r="H217" s="17"/>
       <c r="I217" s="17"/>
     </row>
-    <row r="218" spans="1:9" ht="15.75">
+    <row r="218" spans="1:9" ht="15">
       <c r="A218" s="17"/>
       <c r="B218" s="17" t="s">
         <v>21</v>
@@ -15905,7 +16550,7 @@
       <c r="H218" s="17"/>
       <c r="I218" s="17"/>
     </row>
-    <row r="219" spans="1:9" ht="15.75">
+    <row r="219" spans="1:9" ht="15">
       <c r="A219" s="17"/>
       <c r="B219" s="17" t="s">
         <v>21</v>
@@ -15928,7 +16573,7 @@
       </c>
       <c r="I219" s="17"/>
     </row>
-    <row r="220" spans="1:9" ht="15.75">
+    <row r="220" spans="1:9" ht="15">
       <c r="A220" s="17"/>
       <c r="B220" s="17" t="s">
         <v>21</v>
@@ -15951,7 +16596,7 @@
       </c>
       <c r="I220" s="17"/>
     </row>
-    <row r="221" spans="1:9" ht="15.75">
+    <row r="221" spans="1:9" ht="15">
       <c r="A221" s="17"/>
       <c r="B221" s="17" t="s">
         <v>21</v>
@@ -15974,7 +16619,7 @@
       </c>
       <c r="I221" s="17"/>
     </row>
-    <row r="222" spans="1:9" ht="15.75">
+    <row r="222" spans="1:9" ht="15">
       <c r="A222" s="17"/>
       <c r="B222" s="17" t="s">
         <v>21</v>
@@ -15997,7 +16642,7 @@
       </c>
       <c r="I222" s="17"/>
     </row>
-    <row r="223" spans="1:9" ht="15.75">
+    <row r="223" spans="1:9" ht="15">
       <c r="A223" s="17"/>
       <c r="B223" s="17" t="s">
         <v>21</v>
@@ -16020,7 +16665,7 @@
       </c>
       <c r="I223" s="17"/>
     </row>
-    <row r="224" spans="1:9" ht="15.75">
+    <row r="224" spans="1:9" ht="15">
       <c r="A224" s="17"/>
       <c r="B224" s="17" t="s">
         <v>21</v>
@@ -16043,7 +16688,7 @@
       </c>
       <c r="I224" s="17"/>
     </row>
-    <row r="225" spans="1:9" ht="15.75">
+    <row r="225" spans="1:9" ht="15">
       <c r="A225" s="17"/>
       <c r="B225" s="17" t="s">
         <v>21</v>
@@ -16066,7 +16711,7 @@
       </c>
       <c r="I225" s="17"/>
     </row>
-    <row r="226" spans="1:9" ht="15.75">
+    <row r="226" spans="1:9" ht="15">
       <c r="A226" s="17"/>
       <c r="B226" s="17" t="s">
         <v>21</v>
@@ -16089,7 +16734,7 @@
       </c>
       <c r="I226" s="17"/>
     </row>
-    <row r="227" spans="1:9" ht="15.75">
+    <row r="227" spans="1:9" ht="15">
       <c r="A227" s="17"/>
       <c r="B227" s="17" t="s">
         <v>21</v>
@@ -16112,7 +16757,7 @@
       </c>
       <c r="I227" s="17"/>
     </row>
-    <row r="228" spans="1:9" ht="15.75">
+    <row r="228" spans="1:9" ht="15">
       <c r="A228" s="17"/>
       <c r="B228" s="17" t="s">
         <v>21</v>
@@ -16135,7 +16780,7 @@
       </c>
       <c r="I228" s="17"/>
     </row>
-    <row r="229" spans="1:9" ht="15.75">
+    <row r="229" spans="1:9" ht="15">
       <c r="A229" s="17"/>
       <c r="B229" s="17" t="s">
         <v>21</v>
@@ -16158,7 +16803,7 @@
       </c>
       <c r="I229" s="17"/>
     </row>
-    <row r="230" spans="1:9" ht="15.75">
+    <row r="230" spans="1:9" ht="15">
       <c r="A230" s="17"/>
       <c r="B230" s="17" t="s">
         <v>21</v>
@@ -16181,7 +16826,7 @@
       </c>
       <c r="I230" s="17"/>
     </row>
-    <row r="231" spans="1:9" ht="15.75">
+    <row r="231" spans="1:9" ht="15">
       <c r="A231" s="17"/>
       <c r="B231" s="17" t="s">
         <v>21</v>
@@ -16204,7 +16849,7 @@
       </c>
       <c r="I231" s="17"/>
     </row>
-    <row r="232" spans="1:9" ht="15.75">
+    <row r="232" spans="1:9" ht="15">
       <c r="A232" s="17"/>
       <c r="B232" s="17" t="s">
         <v>21</v>
@@ -16227,7 +16872,7 @@
       </c>
       <c r="I232" s="17"/>
     </row>
-    <row r="233" spans="1:9" ht="15.75">
+    <row r="233" spans="1:9" ht="15">
       <c r="A233" s="17"/>
       <c r="B233" s="17" t="s">
         <v>21</v>
@@ -16250,7 +16895,7 @@
       </c>
       <c r="I233" s="17"/>
     </row>
-    <row r="234" spans="1:9" ht="15.75">
+    <row r="234" spans="1:9" ht="15">
       <c r="A234" s="17" t="b">
         <v>0</v>
       </c>
@@ -16269,7 +16914,7 @@
       <c r="H234" s="17"/>
       <c r="I234" s="17"/>
     </row>
-    <row r="235" spans="1:9" ht="15.75">
+    <row r="235" spans="1:9" ht="15">
       <c r="A235" s="17"/>
       <c r="B235" s="17" t="s">
         <v>21</v>
@@ -16290,7 +16935,7 @@
       <c r="H235" s="17"/>
       <c r="I235" s="17"/>
     </row>
-    <row r="236" spans="1:9" ht="15.75">
+    <row r="236" spans="1:9" ht="15">
       <c r="A236" s="17"/>
       <c r="B236" s="17" t="s">
         <v>21</v>
@@ -16313,7 +16958,7 @@
       </c>
       <c r="I236" s="17"/>
     </row>
-    <row r="237" spans="1:9" ht="15.75">
+    <row r="237" spans="1:9" ht="15">
       <c r="A237" s="17"/>
       <c r="B237" s="17" t="s">
         <v>21</v>
@@ -16336,7 +16981,7 @@
       </c>
       <c r="I237" s="17"/>
     </row>
-    <row r="238" spans="1:9" ht="15.75">
+    <row r="238" spans="1:9" ht="15">
       <c r="A238" s="17"/>
       <c r="B238" s="17" t="s">
         <v>21</v>
@@ -16359,7 +17004,7 @@
       </c>
       <c r="I238" s="17"/>
     </row>
-    <row r="239" spans="1:9" ht="15.75">
+    <row r="239" spans="1:9" ht="15">
       <c r="A239" s="17"/>
       <c r="B239" s="17" t="s">
         <v>21</v>
@@ -16382,7 +17027,7 @@
       </c>
       <c r="I239" s="17"/>
     </row>
-    <row r="240" spans="1:9" ht="15.75">
+    <row r="240" spans="1:9" ht="15">
       <c r="A240" s="17"/>
       <c r="B240" s="17" t="s">
         <v>21</v>
@@ -16405,7 +17050,7 @@
       </c>
       <c r="I240" s="17"/>
     </row>
-    <row r="241" spans="1:9" ht="15.75">
+    <row r="241" spans="1:9" ht="15">
       <c r="A241" s="17"/>
       <c r="B241" s="17" t="s">
         <v>21</v>
@@ -16428,7 +17073,7 @@
       </c>
       <c r="I241" s="17"/>
     </row>
-    <row r="242" spans="1:9" ht="15.75">
+    <row r="242" spans="1:9" ht="15">
       <c r="A242" s="17"/>
       <c r="B242" s="17" t="s">
         <v>21</v>
@@ -16451,7 +17096,7 @@
       </c>
       <c r="I242" s="17"/>
     </row>
-    <row r="243" spans="1:9" ht="15.75">
+    <row r="243" spans="1:9" ht="15">
       <c r="A243" s="17"/>
       <c r="B243" s="17" t="s">
         <v>21</v>
@@ -16474,7 +17119,7 @@
       </c>
       <c r="I243" s="17"/>
     </row>
-    <row r="244" spans="1:9" ht="15.75">
+    <row r="244" spans="1:9" ht="15">
       <c r="A244" s="17"/>
       <c r="B244" s="17" t="s">
         <v>21</v>
@@ -16497,7 +17142,7 @@
       </c>
       <c r="I244" s="17"/>
     </row>
-    <row r="245" spans="1:9" ht="15.75">
+    <row r="245" spans="1:9" ht="15">
       <c r="A245" s="17"/>
       <c r="B245" s="17" t="s">
         <v>21</v>
@@ -16520,7 +17165,7 @@
       </c>
       <c r="I245" s="17"/>
     </row>
-    <row r="246" spans="1:9" ht="15.75">
+    <row r="246" spans="1:9" ht="15">
       <c r="A246" s="17"/>
       <c r="B246" s="17" t="s">
         <v>21</v>
@@ -16543,7 +17188,7 @@
       </c>
       <c r="I246" s="17"/>
     </row>
-    <row r="247" spans="1:9" ht="15.75">
+    <row r="247" spans="1:9" ht="15">
       <c r="A247" s="17"/>
       <c r="B247" s="17" t="s">
         <v>21</v>
@@ -16566,7 +17211,7 @@
       </c>
       <c r="I247" s="17"/>
     </row>
-    <row r="248" spans="1:9" ht="15.75">
+    <row r="248" spans="1:9" ht="15">
       <c r="A248" s="17"/>
       <c r="B248" s="17" t="s">
         <v>21</v>
@@ -16589,7 +17234,7 @@
       </c>
       <c r="I248" s="17"/>
     </row>
-    <row r="249" spans="1:9" ht="15.75">
+    <row r="249" spans="1:9" ht="15">
       <c r="A249" s="17"/>
       <c r="B249" s="17" t="s">
         <v>21</v>
@@ -16612,7 +17257,7 @@
       </c>
       <c r="I249" s="17"/>
     </row>
-    <row r="250" spans="1:9" ht="15.75">
+    <row r="250" spans="1:9" ht="15">
       <c r="A250" s="17"/>
       <c r="B250" s="17" t="s">
         <v>21</v>
@@ -16635,7 +17280,7 @@
       </c>
       <c r="I250" s="17"/>
     </row>
-    <row r="251" spans="1:9" ht="15.75">
+    <row r="251" spans="1:9" ht="15">
       <c r="A251" s="17" t="b">
         <v>0</v>
       </c>
@@ -16654,7 +17299,7 @@
       <c r="H251" s="17"/>
       <c r="I251" s="17"/>
     </row>
-    <row r="252" spans="1:9" ht="15.75">
+    <row r="252" spans="1:9" ht="15">
       <c r="A252" s="17"/>
       <c r="B252" s="17" t="s">
         <v>21</v>
@@ -16679,7 +17324,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="253" spans="1:9" ht="15.75">
+    <row r="253" spans="1:9" ht="15">
       <c r="A253" s="17"/>
       <c r="B253" s="17" t="s">
         <v>21</v>
@@ -16702,7 +17347,7 @@
       </c>
       <c r="I253" s="17"/>
     </row>
-    <row r="254" spans="1:9" ht="15.75">
+    <row r="254" spans="1:9" ht="15">
       <c r="A254" s="17"/>
       <c r="B254" s="17" t="s">
         <v>21</v>
@@ -16725,7 +17370,7 @@
       </c>
       <c r="I254" s="17"/>
     </row>
-    <row r="255" spans="1:9" ht="15.75">
+    <row r="255" spans="1:9" ht="15">
       <c r="A255" s="17"/>
       <c r="B255" s="17" t="s">
         <v>21</v>
@@ -16748,7 +17393,7 @@
       </c>
       <c r="I255" s="17"/>
     </row>
-    <row r="256" spans="1:9" ht="15.75">
+    <row r="256" spans="1:9" ht="15">
       <c r="A256" s="17"/>
       <c r="B256" s="17" t="s">
         <v>21</v>
@@ -16771,7 +17416,7 @@
       </c>
       <c r="I256" s="17"/>
     </row>
-    <row r="257" spans="1:9" ht="15.75">
+    <row r="257" spans="1:9" ht="15">
       <c r="A257" s="17" t="b">
         <v>0</v>
       </c>
@@ -16790,7 +17435,7 @@
       <c r="H257" s="17"/>
       <c r="I257" s="17"/>
     </row>
-    <row r="258" spans="1:9" ht="15.75">
+    <row r="258" spans="1:9" ht="15">
       <c r="A258" s="17"/>
       <c r="B258" s="17" t="s">
         <v>21</v>
@@ -16815,7 +17460,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="259" spans="1:9" ht="15.75">
+    <row r="259" spans="1:9" ht="15">
       <c r="A259" s="17"/>
       <c r="B259" s="17" t="s">
         <v>21</v>
@@ -16838,7 +17483,7 @@
       </c>
       <c r="I259" s="17"/>
     </row>
-    <row r="260" spans="1:9" ht="15.75">
+    <row r="260" spans="1:9" ht="15">
       <c r="A260" s="17" t="b">
         <v>0</v>
       </c>
@@ -16857,7 +17502,7 @@
       <c r="H260" s="17"/>
       <c r="I260" s="17"/>
     </row>
-    <row r="261" spans="1:9" ht="15.75">
+    <row r="261" spans="1:9" ht="15">
       <c r="A261" s="17" t="b">
         <v>0</v>
       </c>
@@ -16876,7 +17521,7 @@
       <c r="H261" s="17"/>
       <c r="I261" s="17"/>
     </row>
-    <row r="262" spans="1:9" ht="15.75">
+    <row r="262" spans="1:9" ht="15">
       <c r="A262" s="17" t="b">
         <v>0</v>
       </c>
@@ -16895,7 +17540,7 @@
       <c r="H262" s="17"/>
       <c r="I262" s="17"/>
     </row>
-    <row r="263" spans="1:9" ht="15.75">
+    <row r="263" spans="1:9" ht="15">
       <c r="A263" s="17"/>
       <c r="B263" s="17" t="s">
         <v>21</v>
@@ -16916,7 +17561,7 @@
       <c r="H263" s="17"/>
       <c r="I263" s="17"/>
     </row>
-    <row r="264" spans="1:9" ht="15.75">
+    <row r="264" spans="1:9" ht="15">
       <c r="A264" s="17"/>
       <c r="B264" s="17" t="s">
         <v>21</v>
@@ -16939,7 +17584,7 @@
       </c>
       <c r="I264" s="17"/>
     </row>
-    <row r="265" spans="1:9" ht="15.75">
+    <row r="265" spans="1:9" ht="15">
       <c r="A265" s="17"/>
       <c r="B265" s="17" t="s">
         <v>21</v>
@@ -16962,7 +17607,7 @@
       </c>
       <c r="I265" s="17"/>
     </row>
-    <row r="266" spans="1:9" ht="15.75">
+    <row r="266" spans="1:9" ht="15">
       <c r="A266" s="17"/>
       <c r="B266" s="17" t="s">
         <v>21</v>
@@ -16985,7 +17630,7 @@
       </c>
       <c r="I266" s="17"/>
     </row>
-    <row r="267" spans="1:9" ht="15.75">
+    <row r="267" spans="1:9" ht="15">
       <c r="A267" s="17"/>
       <c r="B267" s="17" t="s">
         <v>21</v>
@@ -17008,7 +17653,7 @@
       </c>
       <c r="I267" s="17"/>
     </row>
-    <row r="268" spans="1:9" ht="15.75">
+    <row r="268" spans="1:9" ht="15">
       <c r="A268" s="17"/>
       <c r="B268" s="17" t="s">
         <v>21</v>
@@ -17031,7 +17676,7 @@
       </c>
       <c r="I268" s="17"/>
     </row>
-    <row r="269" spans="1:9" ht="15.75">
+    <row r="269" spans="1:9" ht="15">
       <c r="A269" s="17"/>
       <c r="B269" s="17" t="s">
         <v>21</v>
@@ -17054,7 +17699,7 @@
       </c>
       <c r="I269" s="17"/>
     </row>
-    <row r="270" spans="1:9" ht="15.75">
+    <row r="270" spans="1:9" ht="15">
       <c r="A270" s="17"/>
       <c r="B270" s="17" t="s">
         <v>21</v>
@@ -17077,7 +17722,7 @@
       </c>
       <c r="I270" s="17"/>
     </row>
-    <row r="271" spans="1:9" ht="15.75">
+    <row r="271" spans="1:9" ht="15">
       <c r="A271" s="17"/>
       <c r="B271" s="17" t="s">
         <v>21</v>
@@ -17100,7 +17745,7 @@
       </c>
       <c r="I271" s="17"/>
     </row>
-    <row r="272" spans="1:9" ht="15.75">
+    <row r="272" spans="1:9" ht="15">
       <c r="A272" s="17"/>
       <c r="B272" s="17" t="s">
         <v>21</v>
@@ -17123,7 +17768,7 @@
       </c>
       <c r="I272" s="17"/>
     </row>
-    <row r="273" spans="1:9" ht="15.75">
+    <row r="273" spans="1:9" ht="15">
       <c r="A273" s="17"/>
       <c r="B273" s="17" t="s">
         <v>21</v>
@@ -17146,7 +17791,7 @@
       </c>
       <c r="I273" s="17"/>
     </row>
-    <row r="274" spans="1:9" ht="15.75">
+    <row r="274" spans="1:9" ht="15">
       <c r="A274" s="17" t="b">
         <v>0</v>
       </c>
@@ -17165,7 +17810,7 @@
       <c r="H274" s="17"/>
       <c r="I274" s="17"/>
     </row>
-    <row r="275" spans="1:9" ht="15.75">
+    <row r="275" spans="1:9" ht="15">
       <c r="A275" s="17"/>
       <c r="B275" s="17" t="s">
         <v>21</v>
@@ -17188,7 +17833,7 @@
       </c>
       <c r="I275" s="17"/>
     </row>
-    <row r="276" spans="1:9" ht="15.75">
+    <row r="276" spans="1:9" ht="15">
       <c r="A276" s="17" t="b">
         <v>0</v>
       </c>
@@ -17207,7 +17852,7 @@
       <c r="H276" s="17"/>
       <c r="I276" s="17"/>
     </row>
-    <row r="277" spans="1:9" ht="15.75">
+    <row r="277" spans="1:9" ht="15">
       <c r="A277" s="17"/>
       <c r="B277" s="17" t="s">
         <v>21</v>
@@ -17232,7 +17877,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="278" spans="1:9" ht="15.75">
+    <row r="278" spans="1:9" ht="15">
       <c r="A278" s="17"/>
       <c r="B278" s="17" t="s">
         <v>21</v>
@@ -17255,7 +17900,7 @@
       </c>
       <c r="I278" s="17"/>
     </row>
-    <row r="279" spans="1:9" ht="15.75">
+    <row r="279" spans="1:9" ht="15">
       <c r="A279" s="17"/>
       <c r="B279" s="17" t="s">
         <v>21</v>
@@ -17278,7 +17923,7 @@
       </c>
       <c r="I279" s="17"/>
     </row>
-    <row r="280" spans="1:9" ht="15.75">
+    <row r="280" spans="1:9" ht="15">
       <c r="A280" s="17"/>
       <c r="B280" s="17" t="s">
         <v>21</v>
@@ -17301,7 +17946,7 @@
       </c>
       <c r="I280" s="17"/>
     </row>
-    <row r="281" spans="1:9" ht="15.75">
+    <row r="281" spans="1:9" ht="15">
       <c r="A281" s="17"/>
       <c r="B281" s="17" t="s">
         <v>21</v>
@@ -17324,7 +17969,7 @@
       </c>
       <c r="I281" s="17"/>
     </row>
-    <row r="282" spans="1:9" ht="15.75">
+    <row r="282" spans="1:9" ht="15">
       <c r="A282" s="17"/>
       <c r="B282" s="17" t="s">
         <v>21</v>
@@ -17347,7 +17992,7 @@
       </c>
       <c r="I282" s="17"/>
     </row>
-    <row r="283" spans="1:9" ht="15.75">
+    <row r="283" spans="1:9" ht="15">
       <c r="A283" s="17"/>
       <c r="B283" s="17" t="s">
         <v>21</v>
@@ -17370,7 +18015,7 @@
       </c>
       <c r="I283" s="17"/>
     </row>
-    <row r="284" spans="1:9" ht="15.75">
+    <row r="284" spans="1:9" ht="15">
       <c r="A284" s="17"/>
       <c r="B284" s="17" t="s">
         <v>21</v>
@@ -17393,7 +18038,7 @@
       </c>
       <c r="I284" s="17"/>
     </row>
-    <row r="285" spans="1:9" ht="15.75">
+    <row r="285" spans="1:9" ht="15">
       <c r="A285" s="17"/>
       <c r="B285" s="17" t="s">
         <v>21</v>
@@ -17416,7 +18061,7 @@
       </c>
       <c r="I285" s="17"/>
     </row>
-    <row r="286" spans="1:9" ht="15.75">
+    <row r="286" spans="1:9" ht="15">
       <c r="A286" s="17"/>
       <c r="B286" s="17" t="s">
         <v>21</v>
@@ -17439,7 +18084,7 @@
       </c>
       <c r="I286" s="17"/>
     </row>
-    <row r="287" spans="1:9" ht="15.75">
+    <row r="287" spans="1:9" ht="15">
       <c r="A287" s="17"/>
       <c r="B287" s="17" t="s">
         <v>21</v>
@@ -17462,7 +18107,7 @@
       </c>
       <c r="I287" s="17"/>
     </row>
-    <row r="288" spans="1:9" ht="15.75">
+    <row r="288" spans="1:9" ht="15">
       <c r="A288" s="17" t="b">
         <v>0</v>
       </c>
@@ -17481,7 +18126,7 @@
       <c r="H288" s="17"/>
       <c r="I288" s="17"/>
     </row>
-    <row r="289" spans="1:9" ht="15.75">
+    <row r="289" spans="1:9" ht="15">
       <c r="A289" s="17"/>
       <c r="B289" s="17" t="s">
         <v>21</v>
@@ -17504,7 +18149,7 @@
       </c>
       <c r="I289" s="17"/>
     </row>
-    <row r="290" spans="1:9" ht="15.75">
+    <row r="290" spans="1:9" ht="15">
       <c r="A290" s="17" t="b">
         <v>0</v>
       </c>
@@ -17523,7 +18168,7 @@
       <c r="H290" s="17"/>
       <c r="I290" s="17"/>
     </row>
-    <row r="291" spans="1:9" ht="15.75">
+    <row r="291" spans="1:9" ht="15">
       <c r="A291" s="17"/>
       <c r="B291" s="17" t="s">
         <v>21</v>
@@ -17544,7 +18189,7 @@
       <c r="H291" s="17"/>
       <c r="I291" s="17"/>
     </row>
-    <row r="292" spans="1:9" ht="15.75">
+    <row r="292" spans="1:9" ht="15">
       <c r="A292" s="17" t="b">
         <v>0</v>
       </c>
@@ -17563,7 +18208,7 @@
       <c r="H292" s="17"/>
       <c r="I292" s="17"/>
     </row>
-    <row r="293" spans="1:9" ht="15.75">
+    <row r="293" spans="1:9" ht="15">
       <c r="A293" s="17"/>
       <c r="B293" s="17" t="s">
         <v>21</v>
@@ -17584,7 +18229,7 @@
       <c r="H293" s="17"/>
       <c r="I293" s="17"/>
     </row>
-    <row r="294" spans="1:9" ht="15.75">
+    <row r="294" spans="1:9" ht="15">
       <c r="A294" s="17" t="b">
         <v>0</v>
       </c>
@@ -17603,7 +18248,7 @@
       <c r="H294" s="17"/>
       <c r="I294" s="17"/>
     </row>
-    <row r="295" spans="1:9" ht="15.75">
+    <row r="295" spans="1:9" ht="15">
       <c r="A295" s="17"/>
       <c r="B295" s="17" t="s">
         <v>21</v>
@@ -17624,7 +18269,7 @@
       <c r="H295" s="17"/>
       <c r="I295" s="17"/>
     </row>
-    <row r="296" spans="1:9" ht="15.75">
+    <row r="296" spans="1:9" ht="15">
       <c r="A296" s="17" t="b">
         <v>0</v>
       </c>
@@ -17643,7 +18288,7 @@
       <c r="H296" s="17"/>
       <c r="I296" s="17"/>
     </row>
-    <row r="297" spans="1:9" ht="15.75">
+    <row r="297" spans="1:9" ht="15">
       <c r="A297" s="17"/>
       <c r="B297" s="17" t="s">
         <v>21</v>
@@ -17666,7 +18311,7 @@
       </c>
       <c r="I297" s="17"/>
     </row>
-    <row r="298" spans="1:9" ht="15.75">
+    <row r="298" spans="1:9" ht="15">
       <c r="A298" s="17" t="b">
         <v>0</v>
       </c>
@@ -17685,7 +18330,7 @@
       <c r="H298" s="17"/>
       <c r="I298" s="17"/>
     </row>
-    <row r="299" spans="1:9" ht="15.75">
+    <row r="299" spans="1:9" ht="15">
       <c r="A299" s="17"/>
       <c r="B299" s="17" t="s">
         <v>21</v>
@@ -17710,7 +18355,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="300" spans="1:9" ht="15.75">
+    <row r="300" spans="1:9" ht="15">
       <c r="A300" s="17"/>
       <c r="B300" s="17" t="s">
         <v>21</v>
@@ -17733,7 +18378,7 @@
       </c>
       <c r="I300" s="17"/>
     </row>
-    <row r="301" spans="1:9" ht="15.75">
+    <row r="301" spans="1:9" ht="15">
       <c r="A301" s="17"/>
       <c r="B301" s="17" t="s">
         <v>21</v>
@@ -17756,7 +18401,7 @@
       </c>
       <c r="I301" s="17"/>
     </row>
-    <row r="302" spans="1:9" ht="15.75">
+    <row r="302" spans="1:9" ht="15">
       <c r="A302" s="17"/>
       <c r="B302" s="17" t="s">
         <v>21</v>
@@ -17779,7 +18424,7 @@
       </c>
       <c r="I302" s="17"/>
     </row>
-    <row r="303" spans="1:9" ht="15.75">
+    <row r="303" spans="1:9" ht="15">
       <c r="A303" s="17"/>
       <c r="B303" s="17" t="s">
         <v>21</v>
@@ -17802,7 +18447,7 @@
       </c>
       <c r="I303" s="17"/>
     </row>
-    <row r="304" spans="1:9" ht="15.75">
+    <row r="304" spans="1:9" ht="15">
       <c r="A304" s="17"/>
       <c r="B304" s="17" t="s">
         <v>21</v>
@@ -17825,7 +18470,7 @@
       </c>
       <c r="I304" s="17"/>
     </row>
-    <row r="305" spans="1:9" ht="15.75">
+    <row r="305" spans="1:9" ht="15">
       <c r="A305" s="17"/>
       <c r="B305" s="17" t="s">
         <v>21</v>
@@ -17848,7 +18493,7 @@
       </c>
       <c r="I305" s="17"/>
     </row>
-    <row r="306" spans="1:9" ht="15.75">
+    <row r="306" spans="1:9" ht="15">
       <c r="A306" s="17"/>
       <c r="B306" s="17" t="s">
         <v>21</v>
@@ -17871,7 +18516,7 @@
       </c>
       <c r="I306" s="17"/>
     </row>
-    <row r="307" spans="1:9" ht="15.75">
+    <row r="307" spans="1:9" ht="15">
       <c r="A307" s="17"/>
       <c r="B307" s="17" t="s">
         <v>21</v>
@@ -17894,7 +18539,7 @@
       </c>
       <c r="I307" s="17"/>
     </row>
-    <row r="308" spans="1:9" ht="15.75">
+    <row r="308" spans="1:9" ht="15">
       <c r="A308" s="17" t="b">
         <v>0</v>
       </c>
@@ -17913,7 +18558,7 @@
       <c r="H308" s="17"/>
       <c r="I308" s="17"/>
     </row>
-    <row r="309" spans="1:9" ht="15.75">
+    <row r="309" spans="1:9" ht="15">
       <c r="A309" s="17"/>
       <c r="B309" s="17" t="s">
         <v>21</v>
@@ -17936,7 +18581,7 @@
       </c>
       <c r="I309" s="17"/>
     </row>
-    <row r="310" spans="1:9" ht="15.75">
+    <row r="310" spans="1:9" ht="15">
       <c r="A310" s="17"/>
       <c r="B310" s="17" t="s">
         <v>21</v>
@@ -17959,7 +18604,7 @@
       </c>
       <c r="I310" s="17"/>
     </row>
-    <row r="311" spans="1:9" ht="15.75">
+    <row r="311" spans="1:9" ht="15">
       <c r="A311" s="17"/>
       <c r="B311" s="17" t="s">
         <v>21</v>
@@ -17982,7 +18627,7 @@
       </c>
       <c r="I311" s="17"/>
     </row>
-    <row r="312" spans="1:9" ht="15.75">
+    <row r="312" spans="1:9" ht="15">
       <c r="A312" s="17"/>
       <c r="B312" s="17" t="s">
         <v>21</v>
@@ -18005,7 +18650,7 @@
       </c>
       <c r="I312" s="17"/>
     </row>
-    <row r="313" spans="1:9" ht="15.75">
+    <row r="313" spans="1:9" ht="15">
       <c r="A313" s="17" t="b">
         <v>0</v>
       </c>
@@ -18024,7 +18669,7 @@
       <c r="H313" s="17"/>
       <c r="I313" s="17"/>
     </row>
-    <row r="314" spans="1:9" ht="15.75">
+    <row r="314" spans="1:9" ht="15">
       <c r="A314" s="17"/>
       <c r="B314" s="17" t="s">
         <v>21</v>
@@ -18047,7 +18692,7 @@
       </c>
       <c r="I314" s="17"/>
     </row>
-    <row r="315" spans="1:9" ht="15.75">
+    <row r="315" spans="1:9" ht="15">
       <c r="A315" s="17"/>
       <c r="B315" s="17" t="s">
         <v>21</v>
@@ -18070,7 +18715,7 @@
       </c>
       <c r="I315" s="17"/>
     </row>
-    <row r="316" spans="1:9" ht="15.75">
+    <row r="316" spans="1:9" ht="15">
       <c r="A316" s="17"/>
       <c r="B316" s="17" t="s">
         <v>21</v>
@@ -18095,7 +18740,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="317" spans="1:9" ht="15.75">
+    <row r="317" spans="1:9" ht="15">
       <c r="A317" s="17" t="b">
         <v>0</v>
       </c>
@@ -18114,7 +18759,7 @@
       <c r="H317" s="17"/>
       <c r="I317" s="17"/>
     </row>
-    <row r="318" spans="1:9" ht="15.75">
+    <row r="318" spans="1:9" ht="15">
       <c r="A318" s="17"/>
       <c r="B318" s="17" t="s">
         <v>21</v>
@@ -18139,7 +18784,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="319" spans="1:9" ht="15.75">
+    <row r="319" spans="1:9" ht="15">
       <c r="A319" s="17"/>
       <c r="B319" s="17" t="s">
         <v>21</v>
@@ -18162,7 +18807,7 @@
       </c>
       <c r="I319" s="17"/>
     </row>
-    <row r="320" spans="1:9" ht="15.75">
+    <row r="320" spans="1:9" ht="15">
       <c r="A320" s="17" t="b">
         <v>0</v>
       </c>
@@ -18181,7 +18826,7 @@
       <c r="H320" s="17"/>
       <c r="I320" s="17"/>
     </row>
-    <row r="321" spans="1:9" ht="15.75">
+    <row r="321" spans="1:9" ht="15">
       <c r="A321" s="17"/>
       <c r="B321" s="17" t="s">
         <v>21</v>
@@ -18202,7 +18847,7 @@
       <c r="H321" s="17"/>
       <c r="I321" s="17"/>
     </row>
-    <row r="322" spans="1:9" ht="15.75">
+    <row r="322" spans="1:9" ht="15">
       <c r="A322" s="17"/>
       <c r="B322" s="17" t="s">
         <v>21</v>
@@ -18223,7 +18868,7 @@
       <c r="H322" s="17"/>
       <c r="I322" s="17"/>
     </row>
-    <row r="323" spans="1:9" ht="15.75">
+    <row r="323" spans="1:9" ht="15">
       <c r="A323" s="17"/>
       <c r="B323" s="17" t="s">
         <v>21</v>
@@ -18246,7 +18891,7 @@
       </c>
       <c r="I323" s="17"/>
     </row>
-    <row r="324" spans="1:9" ht="15.75">
+    <row r="324" spans="1:9" ht="15">
       <c r="A324" s="17" t="b">
         <v>0</v>
       </c>
@@ -18265,7 +18910,7 @@
       <c r="H324" s="17"/>
       <c r="I324" s="17"/>
     </row>
-    <row r="325" spans="1:9" ht="15.75">
+    <row r="325" spans="1:9" ht="15">
       <c r="A325" s="17" t="b">
         <v>0</v>
       </c>
@@ -18284,7 +18929,7 @@
       <c r="H325" s="17"/>
       <c r="I325" s="17"/>
     </row>
-    <row r="326" spans="1:9" ht="15.75">
+    <row r="326" spans="1:9" ht="15">
       <c r="A326" s="17"/>
       <c r="B326" s="17" t="s">
         <v>21</v>
@@ -18309,7 +18954,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="327" spans="1:9" ht="15.75">
+    <row r="327" spans="1:9" ht="15">
       <c r="A327" s="17"/>
       <c r="B327" s="17" t="s">
         <v>21</v>
@@ -18666,7 +19311,7 @@
       <c r="O343" s="1"/>
       <c r="P343" s="1"/>
     </row>
-    <row r="344" spans="1:16" ht="15.75">
+    <row r="344" spans="1:16" ht="15">
       <c r="A344" s="17"/>
       <c r="B344" t="s">
         <v>21</v>
@@ -19029,7 +19674,7 @@
       <c r="J361"/>
       <c r="K361"/>
     </row>
-    <row r="362" spans="1:18" s="1" customFormat="1" ht="15.75">
+    <row r="362" spans="1:18" s="1" customFormat="1" ht="15">
       <c r="A362" s="17"/>
       <c r="B362" t="s">
         <v>22</v>
@@ -19157,14 +19802,14 @@
       <selection activeCell="A17" sqref="A17:A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" customWidth="1"/>
-    <col min="17" max="17" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" customWidth="1"/>
+    <col min="17" max="17" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">

</xml_diff>